<commit_message>
Update comparison immuannot vs miniport
</commit_message>
<xml_diff>
--- a/results/immuannot_vs_miniprot.xlsx
+++ b/results/immuannot_vs_miniprot.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liuh4\Documents\dash13\dash13-KIR-MHC-assemblies\results\haipeng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4CBAB9E-D58F-4EC2-ABE9-405DD49EB62B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01011DF2-BA54-4CF3-A65C-9CAF71F6695C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{BEB09290-9F4F-4C72-B3D0-BDF1B10BDD9C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{BEB09290-9F4F-4C72-B3D0-BDF1B10BDD9C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="KIR 2DL1 comparison 1" sheetId="1" r:id="rId1"/>
+    <sheet name="KIR 2DL1 comparison 2" sheetId="2" r:id="rId2"/>
+    <sheet name="HLA DRB1 comparison" sheetId="4" r:id="rId3"/>
+    <sheet name="HLA DRB1 miniprot results" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="204">
   <si>
     <t>&gt;KIR2DL1::gene::hg38_tagged::chr19_KI270917v1_alt_hg38_236_159977_0::48259-62999</t>
   </si>
@@ -264,12 +266,444 @@
   <si>
     <t>KIR00001   2DL1*0010101</t>
   </si>
+  <si>
+    <t>HG00733#2#JAHEPP010000060.1_26893186_27481359_1</t>
+  </si>
+  <si>
+    <t>transcript</t>
+  </si>
+  <si>
+    <t>TCACTAATGTGCTTCAGGTATATCCCTGTCTAGAAGTCAGATTGGGGTTAAAGAGTCTGTCCGTGATTGACTAACAGTCTTAAATACTTGATTTGTTGTTGTTGTTGTCCTGTTTGTTTAAGAACTTTACTTCTTTATCCAATGAACGGAGTATCTTGTGTCCTGGACCCTTTGCAAGAACCCTTCCCCTAGCAACAGATGCGTCATCTCAAAATATTTTTCTGATTGGCCAAAGAGTAATTGATTTGCATTTTAATGGTCAGACTCTATTACACCCCACATTCTCTTTTCTTTTATTCTTGTCTGTTCTGCCTCACTCCCGAGCTCTACTGACTCCCAAAAGAGCGCCCAAGAAGAAAATGGCCATAAGTGGAGTCCCTGTGCTAGGATTTTTCATCATAGCTGTGCTGATGAGCGCTCAGGAATCATGGGCTATCAAAGGTAGGTGCTGAGGGAATGAAATCTGGGACGATAGACTACGAAGCATTGGAGAAAAGACCTATGGACATTTGGAAGATAATGTGTGGAGTGAAAGAATAGTGTGACAGGTATTATGTGGTCTCGACAGAAAGTATAACAAATTGTGGTTTGGTGGAGTTCTTCCCTCACCACAAACTGAAGTAAGTCAAATTTGGTTTAGAGGGTCAAAACTGAGTTGTGTATTGATGAATAGCACGGTCCTGCTACAAGCCAAACTGGGGGTGGGGGTGGGGGTGGGGGAGGAAGAATATTTTCTGGCAAGCATTAACAAGTTATATTTCTGGGCTTTAATTATTCTTTCTGGAAAATTAGTAAAATTAAAAACTAAAAACCACACATAGTTTTGCTAGAATTAAATGAAAAAAAAAGTTATTAGCCCTGTTCTTATCTGAATACATGATACAGTAGTTATTTTTTGGAGTGTAAATCCTGTCGGTATATATTGAGCACATATA...</t>
+  </si>
+  <si>
+    <t>ATGGCCATAAGTGGAGTCCCTGTGCTAGGATTTTTCATCATAGCTGTGCTGATGAGCGCTCAGGAATCATGGGCTATCAAAG</t>
+  </si>
+  <si>
+    <t>['gene_id</t>
+  </si>
+  <si>
+    <t>IAG000016.3',</t>
+  </si>
+  <si>
+    <t>'transcript_id</t>
+  </si>
+  <si>
+    <t>IAT000016.3',</t>
+  </si>
+  <si>
+    <t>'gene_name</t>
+  </si>
+  <si>
+    <t>HLA-DRA',</t>
+  </si>
+  <si>
+    <t>'']</t>
+  </si>
+  <si>
+    <t>AAGAACATGTGATCATCCAGGCCGAGTTCTATCTGAATCCTGACCAATCAGGCGAGTTTATGTTTGACTTTGATGGTGATGAGATTTTCCATGTGGATATGGCAAAGAAGGAGACGGTCTGGCGGCTTGAAGAATTTGGACGATTTGCCAGCTTTGAGGCTCAAGGTGCATTGGCCAACATAGCTGTGGACAAAGCCAACCTGGAAATCATGACAAAGCGCTCCAACTATACTCCGATCACCAATG</t>
+  </si>
+  <si>
+    <t>TACCTCCAGAGGTAACTGTGCTCACGAACAGCCCTGTGGAACTGAGAGAGCCCAACGTCCTCATCTGTTTCATCGACAAGTTCACCCCACCAGTGGTCAATGTCACGTGGCTTCGAAATGGAAAACCTGTCACCACAGGAGTGTCAGAGACAGTCTTCCTGCCCAGGGAAGACCACCTTTTCCGCAAGTTCCACTATCTCCCCTTCCTGCCCTCAACTGAGGACGTTTACGACTGCAGGGTGGAGCACTGGGGCTTGGATGAGCCTCTTCTCAAGCACTGGG</t>
+  </si>
+  <si>
+    <t>AGTTTGATGCTCCAAGCCCTCTCCCAGAGACTACAGAGAACGTGGTGTGTGCCCTGGGCCTGACTGTGGGTCTGGTGGGCATCATTATTGGGACCATCTTCATCATCAAGGGAGTGCGCAAAAGCAATGCAGCAGAACGCAGGGGGCCTCTG</t>
+  </si>
+  <si>
+    <t>TCACAATAGCTCCCCAATTAAAGTGTTTTACATGCAACTGGTTCAAACCTTTCAAGTACTAAATTAAAACATTCCTTTAAAGAATGAAATTATTTCAGAAGAGGACCTTCATACAGCATCTCTGAGCAGCAACTGATGATGCTGTTGAACTCAGATGCTGATTGGTTCTCCGACACGAGATTACCCAATCCAGGAGCAAGGAAATCAGTAACTTCCTCCCTATAATTTGGAATGTGGGTGGAGGGGGGTCATAGTTCTCCCTGAGTGAGACTTGCCTGCTCCTCTGGCCCCTGGTCCTGTCCTCTTCTCCAGCATGGTGTGTCTGAAGCTCCCTGGAGGCTCCAGCTTGGCAGCGTTGACAGTGACACTGATGGTGCTGAGCTCCCGACTGGCTTTCGCTGGGGACACCCGACGTAAGAGCACATTGTGGGTGCTGAGCTACTATGGGGTGGGGGAATATAGGGAGTTGTGTTAACATTGTGCCCAGGCCATGTCCCTTAAGAAATTGTGAGGTTTTCTTCAGAGATTGCTCATCTTTATCAAGGGATCGCTAATTATTTCCTCCACAAAAGGAACTTGGCTACTTGCCCTCTCCATGAGACTTGTGTAAGGGGCCTTTGTACAGGCCATTTCTTCTCAAATCTCCACCAATAAAACCTTTGCATCACATGTCCTCAGGGTCTTTAGAGGATTTGGAAATAAGGATGCTAAAATAAATTCCCCAAACAGCAATTCCCTTTATTATGTTGACTTATGTCAGACAAAAGGAGGTTTTTACTGAAAATTTTGTGGGAGTCAAGGGAATTCAATGGGTCTCTCCTAGACGATCCTGGGTTATGTCCTCCACAGGACCTGTGGTGTTGGCCCCTCTTCCTCATATGTGAGGATGGACCCAGTGGCCTCCCTAGTATCTCCTTTCTTTTCTTTCTGAAC...</t>
+  </si>
+  <si>
+    <t>GATTCCTGAGC</t>
+  </si>
+  <si>
+    <t>IAG000019.3',</t>
+  </si>
+  <si>
+    <t>IAT000019.3',</t>
+  </si>
+  <si>
+    <t>HLA-DRB3',</t>
+  </si>
+  <si>
+    <t>GACACTCTGGACTTCAGCCAACAG</t>
+  </si>
+  <si>
+    <t>GTGCACGGTCTGAATCTGCACAGAGCAAGATGCTGAGTGGAGTCGGGGGCTTTGTGCTGGGCCTGCTCTTCCTTGGGGCCGGGCTGTTCATCTACTTCAGGAATCAGAAAG</t>
+  </si>
+  <si>
+    <t>TCCATCCTCAGGTGACTGTGTATCCTGCAAAGACCCAGCCCCTGCAGCACCACAACCTCCTGGTCTGCTCTGTGAGTGGTTTCTATCCAGGCAGCATTGAAGTCAGGTGGTTCCGGAACGGCCAGGAAGAGAAGGCTGGGGTGGTGTCCACGGGCCTGATCCAGAATGGAGACTGGACCTTCCAGACCCTGGTGATGCTAGAAACAGTTCCTCGGAGTGGAGAGGTTTACACCTGCCAAGTGGAGCACCCAAGCGTAACGAGCCCTCTCACAGTGGAATGGA</t>
+  </si>
+  <si>
+    <t>CACGTTTCTTGGAGCTGCTTAAGTCTGAGTGTCATTTCTTCAATGGGACGGAGCGGGTGCGGTTCCTGGAGAGACACTTCCATAACCAGGAGGAGTACGCGCGCTTCGACAGCGACGTGGGGGAGTACCGGGCGGTGAGGGAGCTGGGGCGGCCTGATGCCGAGTACTGGAACAGCCAGAAGGACCTCCTGGAGCAGAAGCGGGGCCAGGTGGACAATTACTGCAGACACAACTACGGGGTTGGTGAGAGCTTCACAGTGCAGCGGCGAG</t>
+  </si>
+  <si>
+    <t>ATGGTGTGTCTGAAGCTCCCTGGAGGCTCCAGCTTGGCAGCGTTGACAGTGACACTGATGGTGCTGAGCTCCCGACTGGCTTTCGCTGGGGACACCCGAC</t>
+  </si>
+  <si>
+    <t>GTGCCTTCATTTCAACTGTGAGACATGATGTAATTTTCACAAATCTACAACAGTAAGATATAGTGCAACAGGACCAGATTAAGGTCTCCTGGTTTGCAACCATGTCCCCTCCATCTCCTTTACTCCTGAACACACTCACTCCTGCAAACAGTTCTCTTGTCAAGTGGGAAATGAATGCTCTTACAAGGCTCAAACTTGTGAACACATCACTGACCAGCACAGAGCTAAAATAATTGGGGCTAAAAATACCGCCCCAATTAAAGTGTTTTACATGCAACTGGTTCAAACCTTTCAAGTACTAAAAACAATCCTGTAAAGAAGGAAATTCTGTTTCAGAAGAGGACCTTCATACAGCATCTCTGACCAGCAACTGATGATGCTATTGAACTCAGATGCTGATTCGTTCTCCAACACTAGATTACCCAATCCAGGAGCAAGGAAATCAGTAACTTACTCCCTATAACTTGGAATGTGGGTGGAGGGGTTCATAGTTCTCCCTGAGTGAGACTTGCCTGCTGCTCTGGCCCCTGGTCCTGTCCTGTTCTCCAGCATGGTGTGTCTGAGGCTCCCTGGAGGCTCCTGCATGGCAGTTCTGACAGTGACACTGATGGTGCTGAGCTCCCCACTGGCTTTGGCTGGGGACACCAGACGTAAGTGCACATTGTGGGTGCTGAGCTACTATGGGGTGGGGAAAATAGGGAGTTTTGTTAACATTGTGCCCAGGCCATGTACCTTAAGAAATTGTGACGTATTTTTCAGAGATTGCCCATCTTTATCATATGGATCCCAAATAATTTCCCCACCACAAAAGGAGCTTGGCTACTTGCCCACTCCATGAGACTTGTGTAAGGGGCCTCCATACAGGTCATTTCTACTCAAATCTCCACCAATAAAACCTTTGCATCACATGTCCTCAGGGTCTTTAGAGGATTT...</t>
+  </si>
+  <si>
+    <t>IAG000017.3',</t>
+  </si>
+  <si>
+    <t>IAT000017.3',</t>
+  </si>
+  <si>
+    <t>HLA-DRB1',</t>
+  </si>
+  <si>
+    <t>GACACTCTGGACTTCAGCCAAGAG</t>
+  </si>
+  <si>
+    <t>GAGCACGGTCTGAATCTGCACAGAGCAAGATGCTGAGTGGAGTCGGGGGCTTTGTGCTGGGCCTGCTCTTCCTTGGGGCCGGGCTGTTCATCTACTTCAGGAATCAGAAAG</t>
+  </si>
+  <si>
+    <t>TCCATCCTAAGGTGACTGTGTATCCTTCAAAGACCCAGCCCCTGCAGCACCATAACCTCCTGGTCTGTTCTGTGAGTGGTTTCTATCCAGGCAGCATTGAAGTCAGGTGGTTCCGGAATGGCCAGGAAGAGAAGACTGGGGTGGTGTCCACAGGCCTGATCCACAATGGAGACTGGACCTTCCAGACCCTGGTGATGCTGGAAACAGTTCCTCGGAGTGGAGAGGTTTACACCTGCCAAGTGGAGCACCCAAGCGTGACAAGCCCTCTCACAGTGGAATGGA</t>
+  </si>
+  <si>
+    <t>CACGTTTCTTGGAGTACTCTACGTCTGAGTGTCATTTCTTCAATGGGACGGAGCGGGTGCGGTACCTGGACAGATACTTCCATAACCAGGAGGAGAACGTGCGCTTCGACAGCGACGTGGGGGAGTTCCGGGCGGTGACGGAGCTGGGGCGGCCTGATGCCGAGTACTGGAACAGCCAGAAGGACCTCCTGGAGCAGAAGCGGGGCCGGGTGGACAACTACTGCAGACACAACTACGGGGTTGTGGAGAGCTTCACAGTGCAGCGGCGAG</t>
+  </si>
+  <si>
+    <t>ATGGTGTGTCTGAGGCTCCCTGGAGGCTCCTGCATGGCAGTTCTGACAGTGACACTGATGGTGCTGAGCTCCCCACTGGCTTTGGCTGGGGACACCAGAC</t>
+  </si>
+  <si>
+    <t>AAAAATTCCTGGAGGTTGTAACTCAGAAAATCCTGAAGGATGCCGTATAATTGATGATGTCATCTATCCACGAGGCTGCTCAGAAATGCCCACCCCTGGCCAGGGCGGTGGCTCATGCCTGTAATCTGAGCACTTTGGGAGGCTGAGATGGGCAGATCACGAATTCAGGAGTTCGAGACCAGCCTGGCCAACATAGTGAAACTCTGTCTCTACTAAAAATACAAAAATTAGCCGGGCGTGGTGGCAGGTGCCTGTAATCCCAGCTACTTGGGAGGGTGAGACAGGAGAATCACTTGAACCCGGGAGTCAAAGTTTGCAGTGAGCCGAGACCATGCCATTGCACCTCAGCCTGGGTGACAGAGTGAGACTACATCTCAAAAAAAAAAAAAAAGAAAGAAAGAAAAAAAGAAAAGAAATGCCCACCCCTCTTGCCACTGGCAGACATGCACACACCAGAGAAGATTCCGATTTCGTGTCCTCCCTCTATTCACAGAACATTTCCTCAAGTCCACTCTGAGTGGAGGCTGCATCACAACAAGGGGATTGCCCTGTCTCCTTCCAGGGCTCTTAATACAAACTCTTCAACTAGTAACTGAGGTGTCATCATAGGGGATTTTTCTAATTAGCCAAAACCTGACTTGGCAGGGTTTGGTTTGGGTGTCTTCAGATTGCCTTGTCTCGAGGTCCTCACAATTGCTCTACAACTCAGAACAGCAACTGCTAAGGCTGCCTTGGGAAGAGGATGATCCTAAACAAAGCTCTGATGCTGGGGGCCCTTGCCCTGACCACCGTGATGAGCCCCTGTGGAGGTGAAGACATTGTGGGTGAGTGTATGAGTGAGGGATGTTCTCTGGAGCTGGAAGAGAGGAAATTGAAGCAAAAGAGAGAAAGCGATTTGCAGAGAAATTGTAGAGATTTCCTAAGGGTCCCTTC...</t>
+  </si>
+  <si>
+    <t>ATGATCCTAAACAAAGCTCTGATGCTGGGGGCCCTTGCCCTGACCACCGTGATGAGCCCCTGTGGAGGTGAAGACATTGTGG</t>
+  </si>
+  <si>
+    <t>IAG000012.3',</t>
+  </si>
+  <si>
+    <t>IAT000012.3',</t>
+  </si>
+  <si>
+    <t>HLA-DQA1',</t>
+  </si>
+  <si>
+    <t>CTGACCACGTCGCCTCTTATGGTGTAAACTTGTACCAGTCTTACGGTCCCTCTGGCCAGTACACCCATGAATTTGATGGAGATGAGCAGTTCTACGTGGACCTGGGGAGGAAGGAGACTGTCTGGTGTTTGCCTGTTCTCAGACAATTTAGATTTGACCCGCAATTTGCACTGACAAACATCGCTGTCCTAAAACATAACTTGAACAGTCTGATTAAACGCTCCAACTCTACCGCTGCTACCAATG</t>
+  </si>
+  <si>
+    <t>AGGTTCCTGAGGTCACAGTGTTTTCCAAGTCTCCCGTGACACTGGGTCAGCCCAACATCCTCATCTGTCTTGTGGACAACATCTTTCCTCCTGTGGTCAACATCACATGGCTGAGCAATGGGCACTCAGTCACAGAAGGTGTTTCTGAGACCAGCTTCCTCTCCAAGAGTGATCATTCCTTCTTCAAGATCAGTTACCTCACCCTCCTCCCTTCTGCTGAGGAGAGTTATGACTGCAAGGTGGAGCACTGGGGCCTGGACAAGCCTCTTCTGAAACACTGGG</t>
+  </si>
+  <si>
+    <t>AGCCTGAGATTCCAGCCCCTATGTCAGAGCTCACAGAGACTGTGGTCTGCGCCCTGGGATTGTCTGTGGGCCTCGTGGGCATTGTGGTGGGCACTGTCTTCATCATCCGAGGCCTGCGTTCAGTTGGTGCTTCCAGACACCAAGGGCCCTTG</t>
+  </si>
+  <si>
+    <t>TTCTAAGAACTTTGCTCTTTTCACCAAAACTTAAGGCTCCTCAGGGTGTGTCTAAGACAACAGCAGTAAAAATGTCTATGACAGCAATTTTCTCTCCCCTGAAATATGATCCCCACTTAATTTGCCCTATTGAAAGAATCCCAAGTATAAGAACAACTGGTTTTTAATCAATATTACAAAGATGTTTACTGTTGAATCGCATTTTTCTTTGGCTTCTTAAAATCCCTTAGGCATTCAATCTTCAGCTCTTCCATAATTGAGAGGAAATTTTCACCTCAAATGTTCATCCAGTGCAATTGAAAGACGTCACAGTGCCAGGCACTGGATTCAGAACCTTCACAAAAAAAAAATCTGCCCAGAGACAGATGAGGTCCTTCAGCTCCAGTGCTGATTGGTTCCTTTCCAAGGGACCATCCAATCCTACCACGCATGGAAACATCCACAGATTTTTATTCTTTCTGCCAGGTACATCAGATCCATCAGGTCCGAGCTGTGTTGACTACCACTTTTCCCTTCGTCTCAATTATGTCTTGGAAAAAGGCTTTGCGGATCCCCGGAGGCCTTCGGGCAGCAACTGTGACCTTGATGCTGTCGATGCTGAGCACCCCAGTGGCTGAGGGCAGAGACTCTCCCGGTAAGTGCAGGGCAGCTGCTCTCCAGAGCCGCTACTCTGGGAACAGGCTCTCCTTGGGCTGGGGTACGGGGATGGTGATCTCCATAATCTCGGACACAATCTTTTATCAACATTTCCTCTGTTTTGGGAAAGAGAGCTATGTTGCATTTCCATTTATCTTTTAATGATGAAGTGAGGACAATCCAATCCCATCCTACAGGCTTAAGCCTGGAAGAGGAGGAGAGAGGAGAGAAAAGAGGAGACAAAGTGTTCATTTACTACCAGTGATAGGACAAAGTGAGCATGGGGTTATTTTTGAA...</t>
+  </si>
+  <si>
+    <t>GGCTCCTGCAC</t>
+  </si>
+  <si>
+    <t>IAG000014.3',</t>
+  </si>
+  <si>
+    <t>IAT000014.3',</t>
+  </si>
+  <si>
+    <t>HLA-DQB1',</t>
+  </si>
+  <si>
+    <t>GGGCTCAATCTGAATCTGCCCAGAGCAAGATGCTGAGTGGCATTGGAGGCTTCGTGCTGGGGCTGATCTTCCTCGGGCTGGGCCTTATCATCCATCACAGGAGTCAGAAAG</t>
+  </si>
+  <si>
+    <t>TGGAGCCCACAGTGACCATCTCCCCATCCAGGACAGAGGCCCTCAACCACCACAACCTGCTGGTCTGCTCGGTGACAGATTTCTATCCAGCCCAGATCAAAGTCCGGTGGTTTCGGAATGACCAGGAGGAGACAGCTGGCGTTGTGTCCACCCCCCTTATTAGGAATGGTGACTGGACCTTCCAGATCCTGGTGATGCTGGAAATGACTCCCCAGCGTGGAGACGTCTACACCTGCCACGTGGAGCACCCCAGCCTCCAGAGCCCCATCACCGTGGAGTGGC</t>
+  </si>
+  <si>
+    <t>AGGATTTCGTGTACCAGTTTAAGGGCATGTGCTACTTCACCAACGGGACAGAGCGCGTGCGTCTTGTGAGCAGAAGCATCTATAACCGAGAAGAGATCGTGCGCTTCGACAGCGACGTGGGGGAGTTCCGGGCGGTGACGCTGCTGGGGCTGCCTGCCGCCGAGTACTGGAACAGCCAGAAGGACATCCTGGAGAGGAAACGGGCGGCGGTGGACAGGGTGTGCAGACACAACTACCAGTTGGAGCTCCGCACGACCTTGCAGCGGCGAG</t>
+  </si>
+  <si>
+    <t>ATGTCTTGGAAAAAGGCTTTGCGGATCCCCGGAGGCCTTCGGGCAGCAACTGTGACCTTGATGCTGTCGATGCTGAGCACCCCAGTGGCTGAGGGCAGAGACTCTCCCG</t>
+  </si>
+  <si>
+    <t>TTCAGATTTGCTTGTCTCGAGGTCCTCACAATTGCTCTGCAGCTCAGAGCAGCAACTGCTGAGGCTGCCTTGGGAAGAAGATGATCCTAAACAAAGCTCTGCTGCTGGGGGCCCTCGCCCTGACTGCCGTGATGAGCCCCTGTGGAGGTGAAGACATTGTGGGTGAGTGCATGAGTGAGGAATGTTCTCTGGAGCTGAAAAACAGTAAATTAAAGGAAAAGAAAGAGTGCAATTTGCTAAGAAATAGTAGAAATTTCCCAAGGGTCTTTTCAATATTAAGAAATTTTAAAATTATGGCAGTTCCTCCTTTAGGAAACCAGAGCTCCAACCGACTCTCTTTGCTACCTGTGCTATTGGAGTTTACCAAGGACGTTGTTCTGTTTATATTATATCCAGAGACTATAGCCTGGAGGTCTGTGTGGCATTCCATCATGATTGCCTCAAAAACTAGGGATGTTTCCATGAATGGAGTATTTTTTTGTTATTAAAAATTTCTGAACTGTTACTCCCAAATTTCTCTGAACAACTTTTGAAGCTTTTCATATGCCTCCTATAGCATATGTTGGGGTAGATAGTTCCATGAAGTATGTACACTCTGTAGATATAAAGAAAGAGGTTCTTTTCTTTCTCTCAGACTTACATTTCCACATGGGAATTGGCACAGGTGGGGAGTAGGTGAAAGAGCCCAGCAGGCTGAATGCCTTCAACAATCATTTTACCACGTGGTAAATGTGGTACTTACTCTCTGCTACCTCATATATGTCACCTCGCTTATGATCAAATAAAATGGGCATGTAGATATGCTTTATGAATAGTAAAAACACGAATGTCAACTTTTTTTAACTTATTTCTATTACAGGTATAACTTCTTATTTTTTCTTTAGCAAAGTAAGGAATATATTTTAAAACTGAGAACTTTATGATAAAATGCT...</t>
+  </si>
+  <si>
+    <t>ATGATCCTAAACAAAGCTCTGCTGCTGGGGGCCCTCGCCCTGACTGCCGTGATGAGCCCCTGTGGAGGTGAAGACATTGTGG</t>
+  </si>
+  <si>
+    <t>IAG000013.3',</t>
+  </si>
+  <si>
+    <t>IAT000013.3',</t>
+  </si>
+  <si>
+    <t>HLA-DQA2',</t>
+  </si>
+  <si>
+    <t>CTGACCATGTTGCCTCCTATGGTGTGAACTTCTACCAGTCTCACGGTCCCTCTGGCCAGTACACCCATGAATTTGATGGAGATGAGGAGTTCTACGTGGACCTGGAGACGAAAGAGACTGTCTGGCAGTTGCCTATGTTTAGCAAATTTATAAGTTTTGACCCGCAGAGTGCACTGAGAAATATGGCTGTGGGAAAACACACCTTGGAATTCATGATGAGACAGTCCAACTCTACCGCTGCCACCAATG</t>
+  </si>
+  <si>
+    <t>AGGTTCCTGAGGTCACAGTGTTTTCCAAGTTTCCTGTGACGCTGGGTCAGCCCAACACCCTCATCTGTCTTGTGGACAACATCTTTCCTCCTGTGGTCAACATCACCTGGCTGAGCAATGGGCACTCAGTCACAGAAGGTGTTTCTGAGACCAGCTTCCTCTCCAAGAGTGATCATTCCTTCTTCAAGATCAGTTACCTCACCTTCCTCCCTTCTGCTGATGAGATTTATGACTGCAAGGTGGAGCACTGGGGCCTGGACGAGCCTCTTCTGAAACACTGGG</t>
+  </si>
+  <si>
+    <t>AGCCTGAGATTCCAGCCCCTATGTCAGAGCTCACAGAGACTTTGGTCTGCGCCCTGGGGTTGTCTGCGGGCCTCATGGGCATTGTGGTGGGCACTGTCTTCATCATCCAAGGCCTGCGTTCAGTTGGTGCTTCCAGACACCAAGGGCTCTTG</t>
+  </si>
+  <si>
+    <t>TCCTTTCCTAGGGACTCCCCAATCCTACCACACATGGAAACATCCAGAGGTTTTTATTCTTTCCGGCAGGTACATAAGATCCATTAGGTTTGAGCTGTGTTGACTACCACTGCTTTTTCCTTGGTCTCACTTATGTCTTGGAAGATGGCTCTGCAGATCCCTGGAGGCTTTTGGGCAGCAGCTGTGACCGTGATGCTGGTGATGCTGAGCACCCCAGTGGCTGAGGCCAGAGACTTTCCCAGTAAGTGCAGGGCAGCTGCTCTCGAGAGCCACCACTGTGGGAACAGGCTCTCCTTGGGTTGGAGTATGGGGGATGGTGATCTCCATGATCTCAGAACACAGTCTTTTATCACCATTTATTCTTTTTGGGAAATAGAGCTATGTTGCATTTTTATTTCCACCTTATAATGGGTGAGGTGAGGATAATCCAACCCCAATCCCACAGGTTTAAGCCTGAAGGAGGAGAGAGGAAAGAGGAGACAAAGTGTGCATTCACTACCTGTGACAGGACAAAATGACCATGGCACTCCACGGTTATGCATTTCCCCAAAGATATGCATTTCCCCAAAGACACAGTAGGATTTTTCTGCACTGGGAAAATGTAAGGCAGCAATGGTGTCTGTAGTCTCTGTATTGGAGGTAAAGGAGTCTATACTACTGACTCGAGTGGAGAGTTTGTGGAGGCAAACTCTTAGTACTGAGGGAAGGTGACTGGATGACCACAGACAGGGAGTCTTACTTTGGGTTTCACTGATTTATGGGCAAAAGGTGACTTGAGTGGGATTCAGGGACCTGAGTTGATGGTGGACTGAATTTAGTATGATAGGAAGGAGGAAGTAAAGAAGGGAAATAATACATATTGAGAAACCACTCCATTCAGACACAGGACAGTACTTTCTATAAATCCTCTCTCACTCCTCCTAACATCCTA...</t>
+  </si>
+  <si>
+    <t>GACTCCTGCAC</t>
+  </si>
+  <si>
+    <t>IAG000015.3',</t>
+  </si>
+  <si>
+    <t>IAT000015.3',</t>
+  </si>
+  <si>
+    <t>HLA-DQB2',</t>
+  </si>
+  <si>
+    <t>GACCTCGAGGGCCTCCACCTGCAG</t>
+  </si>
+  <si>
+    <t>GGGCTCAGTCTGAATCTGCCCAGAGCAAGATGCTGGGTGGTGTTGGAGGCTTCGTGCTGGGGCTGATCTTCCTCGGGCTGGGCCTTATCATCCGTCACAGGGGTCAGAAAG</t>
+  </si>
+  <si>
+    <t>TGGAGCCCACAGTGACCATCTCCCCATCCAGGACAGAGGCCCTCAACCACCACAACCTGCTGGTCTGCTCAGTGACAGATTTCTATCCAGCCCAGATCAAAGTCCAGTGGTTTCGGAATGACCAGGAGGAGACAGCCGGTGTTGTGTCCACCTCCCTCATTAGGAATGGTGACTGGACCTTCCAGATTCTGGTGATGCTGGAAATAACTCCCCAGCGTGGAGACATCTACACCTGCCAAGTGGAGCACCCCAGCCTCCAGAGCCCCATCACCGTGGAGTGGC</t>
+  </si>
+  <si>
+    <t>AGGATTTCTTGGTCCAGTTTAAGGGCATGTGCTACTTCACCAACGGGACAGAGCGCGTGCGGGGTGTGGCCAGATACATCTATAACCGCGAGGAGTACGGGCGCTTCGACAGCGACGTTGGGGAGTTCCAGGCGGTGACCGAGCTGGGGCGGAGCATCGAGGACTGGAACAACTATAAGGACTTCTTGGAGCAGGAGCGGGCCGCGGTGGACAAGGTGTGCAGACACAACTACGAGGCGGAGCTACGCACGACCTTGCAGCGGCAAG</t>
+  </si>
+  <si>
+    <t>ATGTCTTGGAAGATGGCTCTGCAGATCCCTGGAGGCTTTTGGGCAGCAGCTGTGACCGTGATGCTGGTGATGCTGAGCACCCCAGTGGCTGAGGCCAGAGACTTTCCCA</t>
+  </si>
+  <si>
+    <t>CCAGAAAAACAGCGATTTATACTCTTAATGGGTACTTTCTGACTGAATTTTATGAGCTCATTCTGAAGAGGCTGACGATTTTACTATCTCATTTTTTTCCTTTCTCCAGAATGGGTTCTGGGTGGGTCCCCTGGGTGGTGGCTCTGCTAGTGAATCTGACCCGACTGGATTCCTCCATGACTCAAGGCACAGACTCTCCAGGTAAGAACAGAGCAATTGTTTTTTTCCAGTGTGTATGCAAGAATTGGCATGGGGGAGTGATGCCTTTCTTTGTAAGTCCAGGCCACAGACCAGACTGGAAGTGGCTTTTGGTTTCAAAGAACAGTGTTCTTCCCTTTGGCAGAAAGGTACGCCTTGCCTCTTTACATGGGATGGACTTCATATACCAGAGCCACCTATTCAAGGGGTAGGGAGGCAGGAAGAGGGAAACATTGTGTCTTGTTTAGGATCCTTATTGTGTGTATCAACCTCAGTCAGTGCCTGGGCGTGTTGAAGGCCTTGGCTTGGGTTCGAGCCTGCTGGGAGAAACAACCTGCAGTAGGCTGGGTCACAGAGGCAATCTGTGATTTTTTGGTCAGGACACGGAAACAAATCTCAGTTGGGGTATATGTGGACAAATGAAACTGGAAACAAAGGTTGCTCCTTCTGTCATTTATTAAGCCACTATTATATTGTCAGAATTGTACTAAACAGTTTTGAGAAGTAAGAGAAGTTGAATAGAATACATTGTCCTTGTCCTCCGGCTACCAGGTACAAGTTACTTGTCACTGTTATTTTTCTAGCACAGGTGACAGAATATGCAGCCATGAAGCAATGTGAGATGAAAGCACATATTAATGAGCAGAAACAGGATGTAATGTGCTAAGAACAGAATCCCCTTTGCATGTTAGTTTCATTAAATACAAAAGAGGAACAAACCTGGCCAGGAGAG...</t>
+  </si>
+  <si>
+    <t>GTCTCAAGAGCTGTTCTGCTCCCTCAGTCATGC</t>
+  </si>
+  <si>
+    <t>IAG000007.3',</t>
+  </si>
+  <si>
+    <t>IAT000007.3',</t>
+  </si>
+  <si>
+    <t>HLA-DOB',</t>
+  </si>
+  <si>
+    <t>GATATGTGAGGACGCAGATGTCTGGTAATGAG</t>
+  </si>
+  <si>
+    <t>GAGCTCAGTCTGAATATTCTTGGAGAAAGATGCTGAGTGGCATTGCAGCCTTCCTACTTGGGCTAATCTTCCTTCTGGTGGGAATCATCATCCAGCTAAGGGCTCAGAAAG</t>
+  </si>
+  <si>
+    <t>TGCAACCAGAGGTGACAGTGTACCCAGAGAGGACCCCACTCCTGCACCAGCATAATCTGCTGCACTGCTCTGTGACAGGCTTCTATCCAGGGGATATCAAGATCAAGTGGTTCCTGAATGGGCAGGAGGAGAGAGCTGGGGTCATGTCCACTGGCCCTATCAGGAATGGAGACTGGACCTTTCAGACTGTGGTGATGCTAGAAATGACTCCTGAACTTGGACATGTCTACACCTGCCTTGTCGATCACTCCAGCCTGCTGAGCCCTGTTTCTGTGGAGTGGA</t>
+  </si>
+  <si>
+    <t>AAGATTTTGTGATTCAGGCAAAGGCTGACTGTTACTTCACCAACGGGACAGAAAAGGTGCAGTTTGTGGTCAGATTCATCTTTAACTTGGAGGAGTATGTACGTTTCGACAGTGATGTGGGGATGTTTGTGGCATTGACCAAGCTGGGGCAGCCAGATGCTGAGCAGTGGAACAGCCGGCTGGATCTCTTGGAGAGGAGCAGACAGGCCGTGGATGGGGTCTGTAGACACAACTACAGGCTGGGCGCACCCTTCACTGTGGGGAGAAAAG</t>
+  </si>
+  <si>
+    <t>ATGGGTTCTGGGTGGGTCCCCTGGGTGGTGGCTCTGCTAGTGAATCTGACCCGACTGGATTCCTCCATGACTCAAGGCACAGACTCTCCAG</t>
+  </si>
+  <si>
+    <t>ACAAAGCAAGGACAACAGATAAAGTTGCCCTTGAGACAACTGTATTTTACTTAATGATAAAGAAACATTTTTGCAGTTTTATATCCCAGAGTAACCGCCACTAAAGGCGAGTGAGACTCATTGCAGGCCTGTACAGTGCGAACCAGAGTTCGGGCTCCAGTTCCGCTGTCTGCGGGTCTCGCGCGCCCCCTCCCGGCGGCCCAGCCCAGAATGAAGGCCTTGGCTGGGGAAGCGAAAGCGAAAGCTGCCCGAGCCCTGACGCCCGCCCTGGCCGAGCGTAGCTGGCGGACCAGAGCCGGTAGCGAGGTTGGGAGAGACGGAGCGGACCTCAGCGCTGAAGCAGAAGTCCCCGGAGCTGCGGTCTCCCCGCCGCGGCTGGTGAGTTGGTGCGGAGGGGAACCTGGAGCGCCAACAGGGACGCAGCCCAAGTGACTACCCACTCCACGCTCCTGCTTCCCAGTCCCTCTGCACCCGGCGATAGGAGGGAGCGGAGCCCGGACCACTTAGCTCGCCGCGGCAGGCGGGGGTGGGGGTGGGGGTCCGGGGATTTTTTTTTTTTTTTTTTTAAGCACGAGGCTCCTGATGGTCATGCTTCCAGCTCCCCAGAAGGCCGAAAGCTGTCTGTCGTAGGAGGGGTGTACGGATGAGCACCGGTTACTCAGGAGAGCTCTCAGGGTTGAATAGGATAAAATGAGAAGCCGATGGACGGGTTAGGCGGAGCCGGGCGGGTAGGAGGGCAGGGACAAGGATTGGGACTCCACCCCCATGATTTCTCATCTCGTATCCGTTGACAGAGCCATGCGGCTCCCTGACCTGAGACCCTGGACCTCCCTGCTGCTGGTGGACGCGGCTTTACTGTGGCTGCTTCAGGGCCCTCTGGGGACTTTGCTTCCTCAAGGGCTGCCAGGACTATGGCTGGAGGGGACCCTGC...</t>
+  </si>
+  <si>
+    <t>CTGCAGGACTGGAATTCCCGTGGGGATCGCACAGTGCTGGTGATTGCTCACAGGCTGCAGACAGTTCAGCGCGCCCACCAGATCCTGGTGCTCCAGGAGGGCAAGCTGCAGAAGCTTGCCCAGCTC</t>
+  </si>
+  <si>
+    <t>IAG000062.3',</t>
+  </si>
+  <si>
+    <t>IAT000062.3',</t>
+  </si>
+  <si>
+    <t>TAP2',</t>
+  </si>
+  <si>
+    <t>ATGTAGGGGAGAAGGGAAGCCAGCTGGCTGCGGGACAGAAACAACGTCTGGCCATTGCCCGGGCCCTTGTACGAGACCCGCGGGTCCTCATCCTGGATGAGGCTACTAGTGCCCTAGATGTGCAGTGCGAGCAGGCC</t>
+  </si>
+  <si>
+    <t>GTGGTTTCAGTTGGGCAGGAGCCTGTGCTGTTCTCCGGTTCTGTGAGGAACAACATTGCTTATGGGCTGCAGAGCTGCGAAGATGATAAGGTGATGGCGGCTGCCCAGGCTGCCCACGCAGATGACTTCATCCAGGAAATGGAGCATGGAATATACACAG</t>
+  </si>
+  <si>
+    <t>GGGCTGACGTTTACCCTACGTCCTGGTGAGGTGACGGCGCTGGTGGGACCCAATGGGTCTGGGAAGAGCACAGTGGCTGCCCTGCTGCAGAATCTGTACCAGCCCACAGGGGGACAGGTGCTGCTGGATGAAAAGCCCATCTCACAGTATGAACACTGCTACCTGCACAGCCAG</t>
+  </si>
+  <si>
+    <t>ACCCTGGTATACATATATGGGGATATGCTCAGCAACGTGGGAGCTGCAGAGAAGGTTTTCTCCTACATGGACCGACAGCCAAATCTGCCTTCACCTGGCACGCTTGCCCCCACCACTCTGCAGGGGGTTGTGAAATTCCAAGACGTCTCCTTTGCATATCCCAATCGCCCTGACAGGCCTGTGCTCAAG</t>
+  </si>
+  <si>
+    <t>GTGCTGCACTTGGGGGTGCAGATGCTGATGCTGAGCTGTGGGCTGCAGCAGATGCAGGATGGGGAGCTCACCCAGGGCAGCCTGCTTTCCTTTATGATCTACCAGGAGAGCGTGGGGAGCTATGTGCAG</t>
+  </si>
+  <si>
+    <t>GAAGTGCTTCGGGAGATCCAGGATGCAGTGGCCAGGGCGGGGCAGGTGGTGCGGGAAGCCGTTGGAGGGCTGCAGACCGTTCGCAGTTTTGGGGCCGAGGAGCATGAAGTCTGTCGCTATAAAGAGGCCCTTGAACAATGTCGGCAGCTGTATTGGCGGAGAGACCTGGAACGCGCCTTGTACCTGCTCGTAAGGAGG</t>
+  </si>
+  <si>
+    <t>GGGAGCTGAACTCACGGCTGAGCTCGGATACCACCCTGATGAGTAACTGGCTTCCTTTAAATGCCAATGTGCTCTTGCGAAGCCTGGTGAAAGTGGTGGGGCTGTATGGCTTCATGCTCAGCATATCGCCTCGACTCACCCTCCTTTCTCTGCTGCACATGCCCTTCACAATAGCAGCGGAGAAGGTGTACAACACCCGCCATCAG</t>
+  </si>
+  <si>
+    <t>CTCACTGTCTGCAGGCTGCCGAGGAGGCTGCTTCACCTACACCATGTCTCGAATCAACTTGCGGATCCGGGAGCAGCTTTTCTCCTCCCTGCTGCGCCAGGACCTCGGTTTCTTCCAGGAGACTAAGACAG</t>
+  </si>
+  <si>
+    <t>GTGAGACATTAATCCCTCACTATTCTGGTCGTGTGATTGACATCCTGGGAGGTGATTTTGACCCCCATGCCTTTGCCAGTGCCATCTTCTTCATGTGCCTCTTCTCCTTTGGCAG</t>
+  </si>
+  <si>
+    <t>ATGCGGCTCCCTGACCTGAGACCCTGGACCTCCCTGCTGCTGGTGGACGCGGCTTTACTGTGGCTGCTTCAGGGCCCTCTGGGGACTTTGCTTCCTCAAGGGCTGCCAGGACTATGGCTGGAGGGGACCCTGCGGCTGGGAGGGCTGTGGGGGCTGCTAAAGCTAAGAGGGCTGCTGGGATTTGTGGGGACACTGCTGCTCCCGCTCTGTCTGGCCACCCCCCTGACTGTCTCCCTGAGAGCCCTGGTCGCGGGGGCCTCACGTGCTCCCCCAGCCAGAGTCGCTTCAGCCCCTTGGAGCTGGCTGCTGGTGGGGTACGGGGCTGCGGGGCTCAGCTGGTCACTGTGGGCTGTTCTGAGCCCTCCTGGAGCCCAGGAGAAGGAGCAGGACCAGGTGAACAACAAAGTCTTGATGTGGAGGCTGCTGAAGCTCTCCAGGCCGGACCTGCCTCTCCTCGTTGCCGCCTTCTTCTTCCTTGTCCTTGCTGTTTTGG</t>
+  </si>
+  <si>
+    <t>CCTGCAAGGCACCGCTCTCCTCGCCGCCTGGGGCACTGGTTTCCAACCTGGGACAGCGCACAACGCGCAGCCGACAGCCCCGCCCCTTCGCGGCGCCGCCAGGAGGCGCCTGGGTGCTGCGGGGCTGCTTTGCGCGCGGCGCTAACGTGTGTAGGGCAGATCTGCCCCGAGACAAGTGACGAGGCAGCCCCGCCCTGAGGCTGGGGTGGGAAAACTGGTGCAAGTGGAAAGGCAGGAGGCAGGGAGAGGCGAGAAGGGTGTGCGTGATGGAGAAAATTGGGCACCAGGGCTGCTCCCGAGATTCTCAGATCTGATTTCCACGCTTGCTACCAAAATAGTCTGGGCAGGCCACTTTTGGAAGTAGGCGTTATCTAGTGAGCAGGCGGCCGCTTTCGATTTCGCTTTCCCCTAAATGGCTGAGCTTCTCGCCAGCGCAGGATCAGCCTGTTCCTGGGACTTTCCGAGAGCCCCGCCCTCGTTCCCTCCCCCAGCCGCCAGTAGGGGAGGACTCGGCGGTACCCGGAGCTTCAGGCCCCACCGGGGCGCGGAGAGTCCCAGGCCCGGCCGGGACCGGGACGGCGTCCGAGTGCCAATGGCTAGCTCTAGGTGTCCCGCTCCCCGCGGGTGCCGCTGCCTCCCCGGAGCTTCTCTCGCATGGCTGGGGACAGTACTGCTACTTCTCGCCGACTGGGTGCTGCTCCGGACCGCGCTGCCCCGCATATTCTCCCTGCTGGTGCCCACCGCGCTGCCACTGCTCCGGGTCTGGGCGGTGGGCCTGAGCCGCTGGGCCGTGCTCTGGCTGGGGGCCTGCGGGGTCCTCAGGGCAACGGTTGGCTCCAAGAGCGAAAACGCAGGTGCCCAGGGCTGGCTGGCTGCTTTGAAGCCATTAGCTGCGGCACTGGGCTTGGCCCTGCCGGGACTTGCCTTGTTC...</t>
+  </si>
+  <si>
+    <t>GTGGAGCAGCTCCTGTACGAAAGCCCTGAGCGGTACTCCCGCTCAGTGCTTCTCATCACCCAGCACCTCAGCCTGGTGGAGCAGGCTGACCACATCCTCTTTCTGGAAGGAGGCGCTATCCGGGAGGGGGGAACCCACCAGCAGCTCATGGAGAAAAAGGGGTGCTACTGGGCCATGGTGCAGGCTCCTGCAGATGCTCCAGAA</t>
+  </si>
+  <si>
+    <t>IAG000061.3',</t>
+  </si>
+  <si>
+    <t>IAT000061.3',</t>
+  </si>
+  <si>
+    <t>TAP1',</t>
+  </si>
+  <si>
+    <t>AGGTAGACGAGGCTGGGAGCCAGCTGTCAGGGGGTCAGCGACAGGCAGTGGCGTTGGCCCGAGCATTGATCCGGAAACCGTGTGTACTTATCCTGGATGATGCCACCAGTGCCCTGGATGCAAACAGCCAGTTACAG</t>
+  </si>
+  <si>
+    <t>GTGGCTGCAGTGGGACAAGAGCCACAGGTATTTGGAAGAAGTCTTCAAGAAAATATTGCCTATGGCCTGACCCAGAAGCCAACTATGGAGGAAATCACAGCTGCTGCAGTAAAGTCTGGGGCCCATAGTTTCATCTCTGGACTCCCTCAGGGCTATGACACAG</t>
+  </si>
+  <si>
+    <t>GGGCTGACATTCACCCTACGCCCTGGCGAGGTGACGGCGCTGGTGGGACCCAATGGGTCTGGGAAGAGCACAGTGGCTGCCCTGCTGCAGAATCTGTACCAGCCCACCGGGGGACAGCTGCTGTTGGATGGGAAGCCCCTTCCCCAATATGAGCACCGCTACCTGCACAGGCAG</t>
+  </si>
+  <si>
+    <t>GTACTGCTCTCCATCTACCCCAGAGTACAGAAGGCTGTGGGCTCCTCAGAGAAAATATTTGAGTACCTGGACCGCACCCCTCGCTGCCCACCCAGTGGTCTGTTGACTCCCTTACACTTGGAGGGCCTTGTCCAGTTCCAAGATGTCTCCTTTGCCTACCCAAACCGCCCAGATGTCTTAGTGCTACAG</t>
+  </si>
+  <si>
+    <t>ATTTCAGGTATGCTGCTGAAAGTGGGAATCCTCTACATTGGTGGGCAGCTGGTGACCAGTGGGGCTGTAAGCAGTGGGAACCTTGTCACATTTGTTCTCTACCAGATGCAGTTCACCCAGGCTGTGGAG</t>
+  </si>
+  <si>
+    <t>TTGCTGGAAGTGCAGGTGCGGGAATCTCTGGCAAAGTCCAGCCAGGTGGCCATTGAGGCTCTGTCGGCCATGCCTACAGTTCGAAGCTTTGCCAACGAGGAGGGCGAAGCCCAGAAGTTTAGGGAAAAGCTGCAAGAAATAAAGACACTCAACCAGAAGGAGGCTGTGGCCTATGCAGTCAACTCCTGGACCACTAGT</t>
+  </si>
+  <si>
+    <t>GTAACATCATGTCTCGGGTAACAGAGGACACGTCCACCCTGAGTGATTCTCTGAGTGAGAATCTGAGCTTATTTCTGTGGTACCTGGTGCGAGGCCTATGTCTCTTGGGGATCATGCTCTGGGGATCAGTGTCCCTCACCATGGTCACCCTGATCACCCTGCCTCTGCTTTTCCTTCTGCCCAAGAAGGTGGGAAAATGGTACCAG</t>
+  </si>
+  <si>
+    <t>TGCAGTGCTGGAGTTCGTGGGTGACGGGATCTATAACAACACCATGGGCCACGTGCACAGCCACTTGCAGGGAGAGGTGTTTGGGGCTGTCCTGCGCCAGGAGACGGAGTTTTTCCAACAGAACCAGACAG</t>
+  </si>
+  <si>
+    <t>GGGAGATGGCCATTCCATTCTTTACGGGCCGCCTCACTGACTGGATTCTACAAGATGGCTCAGCCGATACCTTCACTCGAAACTTAACTCTCATGTCCATTCTCACCATAGCCAG</t>
+  </si>
+  <si>
+    <t>ATGGCTAGCTCTAGGTGTCCCGCTCCCCGCGGGTGCCGCTGCCTCCCCGGAGCTTCTCTCGCATGGCTGGGGACAGTACTGCTACTTCTCGCCGACTGGGTGCTGCTCCGGACCGCGCTGCCCCGCATATTCTCCCTGCTGGTGCCCACCGCGCTGCCACTGCTCCGGGTCTGGGCGGTGGGCCTGAGCCGCTGGGCCGTGCTCTGGCTGGGGGCCTGCGGGGTCCTCAGGGCAACGGTTGGCTCCAAGAGCGAAAACGCAGGTGCCCAGGGCTGGCTGGCTGCTTTGAAGCCATTAGCTGCGGCACTGGGCTTGGCCCTGCCGGGACTTGCCTTGTTCCGAGAGCTGATCTCATGGGGAGCCCCCGGGTCCGCGGATAGCACCAGGCTACTGCACTGGGGAAGTCACCCTACCGCCTTCGTTGTCAGTTATGCAGCGGCACTGCCCGCAGCAGCCCTGTGGCACAAACTCGGGAGCCTCTGGGTGCCCGGCGGTCAGGGCGGCTCTGGAAACCCTGTGCGTCGGCTTCTAGGCTGCCTGGGCTCGGAGACGCGCCGCCTCTCGCTGTTCCTGGTCCTGGTGGTCCTCTCCTCTCTTG</t>
+  </si>
+  <si>
+    <t>GAGCAGAGCATGATCACATTCCTGCCGCTGCTGCTGGGGCTCAGCCTGGGCTGCACAGGAGCAGGTAAGGACACTTCTTCTGGGGACTCTCCCTTCCCCTGCTCCTGTTTCAGGGTAAGGGTGTTCCGTTTTGTAATTGCATTTGACACCCCAGATAGTTTGTCTCCCTGGTATACATTCCTATAGCACTTTGTACTTTGTAGCAATTTTAATGTAATTAATCTGTATAATTATCTGTGCAGTGTATATTCCCTGCTGGAATATAGGCAAGGACAATGTTCATCTTATTTATTGCTGCCTCCTCAGCTCCTAGCACAGTGCCTTGCATGCAGCAAGTGCTTCATAAATATGTGCGAAGTGAATATTTAATATTTCCAGCACAATACAAGGCTGACTCTTTCTCTTGACCCTTTTTCTCTCTCAATAATTTGCCTTACTGAAGGTCTGTGTTCTGGGCAAATTGTCATGTTTAAACATGCAAATAATCTCGGGGGGCTACTCCTATCCCTGTGCTTAGTCTTGCATAAAGAGGAGACTGGATCTAAAAACTTATCTACTACTTCTACTGACTCCCTCAAATCAGACTTTCAGAAACTTCAGTGTATGAGCTTGGTCAGTAGATGTTCCCTGAGCAGGAAATCTGTGCCAGACTAGCTGGATGTCACCAAGGCTTAGGTTCTGAGCTGAATATAGGAAAAATCAACTTTTTTTCTTCTATATGCTCACACTCAACACTTCTTTGACCAACTGTGTGAGGTTTTTTTTTTTTTTTTACTCATACCAACCAATTCTCCTATATTAGCTGGATATCCTATAATTCAATTCCATTGTGACATTAACTAGAGTTAACATAGACACCAAAGGTTAAAGACTCAGTCCCATAAGACTGCCTCCATTTCAGACACCAATCACAAGTAGTAGGTTCCCAAAT...</t>
+  </si>
+  <si>
+    <t>GATGGCACATTTCC</t>
+  </si>
+  <si>
+    <t>IAG000005.3',</t>
+  </si>
+  <si>
+    <t>IAT000005.3',</t>
+  </si>
+  <si>
+    <t>HLA-DMB',</t>
+  </si>
+  <si>
+    <t>GTTACACTCCTCTTCCTGGGTCCAATTATTCAGAAG</t>
+  </si>
+  <si>
+    <t>CACCTGGGCTGTCCCCCATGCAGACCCTGAAGGTTTCTGTGTCTGCAGTGACTCTGGGCCTGGGCCTCATCATCTTCTCTCTTGGTGTGATCAGCTGGCGGAGAGCTGGCCACTCTA</t>
+  </si>
+  <si>
+    <t>GGCCACCATCTGTGCAAGTAGCCAAAACCACTCCTTTTAACACGAGGGAGCCTGTGATGCTGGCCTGCTATGTGTGGGGCTTCTATCCAGCAGAAGTGACTATCACGTGGAGGAAGAACGGGAAGCTTGTCATGCCTCACAGCAGTGTGCACAAGACTGCCCAGCCCAATGGAGACTGGACATACCAGACCCTCTCCCATTTAGCCTTAACCCCCTCTTACGGGGACACTTACACCTGTGTGGTAGAGCACACTGGGGCTCCTGAGCCCATCCTTCGGGACTGGA</t>
+  </si>
+  <si>
+    <t>GTGGCTTCGTGGCCCATGTGGAAAGCACCTGTCTGTTGGATGATGCTGGGACTCCAAAGGATTTCACATACTGCATCTCCTTCAACAAGGATCTGCTGACCTGCTGGGATCCAGAGGAGAATAAGATGGCCCCTTGCGAATTTGGGGTGCTGAATAGCTTGGCGAATGTCCTCTCACAGCACCTCAACCAAAAAGACACCCTGATGCAGCGCTTGCGCAATGGGCTTCAGAATTGTGCCACACACACCCAGCCCTTCTGGGGATCACTGACCAACAGGACAC</t>
+  </si>
+  <si>
+    <t>ATGATCACATTCCTGCCGCTGCTGCTGGGGCTCAGCCTGGGCTGCACAGGAGCAG</t>
+  </si>
+  <si>
+    <t>CTGACAGCTTGAAACCAAAGAGGGAACTCCACCAGGAAGCAACATTCCTCCACTGGGCTTCCCAGCCCAGTTACATGCCATACTCTGCCCTGGTCAAACAGCCAAGTCTTCAGGAGGTTACTGGCCCCAGGCGTCTCCCCAGTGACTGATGATGTTAAACCCTACGCTTCTCTGATTGGTTTAGACAAAATGACAAGGGCACCTATTGGAAATGATCTGGCAAAACATGATCTAAGGCCACCCTCTCGGGGAGGGAGTTGGGGAAGCTGGGTTGGCTGGGTTGGTAGCTCCTACCTACTGTGTGGCAAGAAGGTATGGGTCATGAACAGAACCAAGGAGCTGCGCTGCTACAGATGTTACCACTTCTGTGGCTGCTACCCCACTCCTGGGCCGTCCCTGAAGGTAAGATGGTACTCCTATTTACTTCCATCCTGAACCTAGGGAGCCCACTCAGCTTTGTGAGGAAAAGCGCTGTGCTTTGTGAGTGGTGGGAAGTCTTATGAGGCAGTGGAAACAACAGGGGAGTGGGGAAAGACAGCTGCTATGTGTGGTTGGTAAACGATATCAGTGATGCTTTGCATGTTCCATTTAAGACAATCTCTTGAAGCGGAGATTGTTCTCTCCATTTTACAAATGAAGAAAATGAGACTCAGAGTTATTTGTGCAAGTTCACACCATTGGAAAGTGGTAGAGCTGGGATTTGAACAAAGTGAATGTTATTTTCACTCCTCCACTCAAGATTCTACTCTGCTTTCTATCATTAACTTATCTTGTGATTCTTGAAAAGTGTCTTAGTTTCCTTCTCTGTAGAGGATGGGGCAGAATGGAAGAATAATCTGGAAGATCCCTCTTCCTCCAAATGTCTGTTTTTCTGGGTATTGGGTTAAAGGTTTCCTGCTGGCTGAGCGATTCCTGCCAAGAGCTTCAAAGA...</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>IAG000004.3',</t>
+  </si>
+  <si>
+    <t>IAT000004.3',</t>
+  </si>
+  <si>
+    <t>HLA-DMA',</t>
+  </si>
+  <si>
+    <t>TACCCCGGAACGCACTGCCCTCAGATCTGCTGGAGAATGTGCTGTGTGGCGTGGCCTTTGGCCTGGGTGTGCTGGGCATCATCGTGGGCATTGTTCTCATCATCTACTTCCGGAAGCCTTGCTCAGGTG</t>
+  </si>
+  <si>
+    <t>GGTTTCCTATCGCTGAAGTGTTCACGCTGAAGCCCCTGGAGTTTGGCAAGCCCAACACTTTGGTCTGTTTTGTCAGTAATCTCTTCCCACCCATGCTGACAGTGAACTGGCAGCATCATTCCGTCCCTGTGGAAGGATTTGGGCCTACTTTTGTCTCAGCTGTCGATGGACTCAGCTTCCAGGCCTTTTCTTACTTAAACTTCACACCAGAACCTTCTGACATTTTCTCCTGCATTGTGACTCACGAAATTGACCGCTACACAGCAATTGCCTATTGGG</t>
+  </si>
+  <si>
+    <t>CTCCTACTCCAATGTGGCCAGATGACCTGCAAAACCACACATTCCTGCACACAGTGTACTGCCAGGATGGGAGTCCCAGTGTGGGACTCTCTGAGGCCTACGACGAGGACCAGCTTTTCTTCTTCGACTTTTCCCAGAACACTCGGGTGCCTCGCCTGCCCGAATTTGCTGACTGGGCTCAGGAACAGGGAGATGCTCCTGCCATTTTATTTGACAAAGAGTTCTGCGAGTGGATGATCCAGCAAATAGGGCCAAAACTTGATGGGAAAATCCCGGTGTCCAGAG</t>
+  </si>
+  <si>
+    <t>ATGGGTCATGAACAGAACCAAGGAGCTGCGCTGCTACAGATGTTACCACTTCTGTGGCTGCTACCCCACTCCTGGGCCGTCCCTGAAG</t>
+  </si>
+  <si>
+    <t>&gt;HLA-DRB1</t>
+  </si>
+  <si>
+    <t>184201-198070</t>
+  </si>
+  <si>
+    <t>184201-184524</t>
+  </si>
+  <si>
+    <t>184201-184538</t>
+  </si>
+  <si>
+    <t>184524-184527</t>
+  </si>
+  <si>
+    <t>184527-184538</t>
+  </si>
+  <si>
+    <t>185326-185350</t>
+  </si>
+  <si>
+    <t>185825-185936</t>
+  </si>
+  <si>
+    <t>186634-186916</t>
+  </si>
+  <si>
+    <t>189156-189426</t>
+  </si>
+  <si>
+    <t>197420-197520</t>
+  </si>
+  <si>
+    <t>197420-198070</t>
+  </si>
+  <si>
+    <t>197517-197520</t>
+  </si>
+  <si>
+    <t>197520-198070</t>
+  </si>
+  <si>
+    <t>Same as below with 1 number shift</t>
+  </si>
+  <si>
+    <t>HLA-C2-KIR_gene_feature_sequences_from_immuannot\HLA-DRB1_features.fa</t>
+  </si>
+  <si>
+    <t>HLA_gene_features_by_miniprot\HLA_ClassII_feature_seq.txt</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,6 +722,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -325,11 +766,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -813,8 +1255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8272538C-7265-40CB-9F5A-05785FE88769}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1301,4 +1743,3804 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAAF866E-C67C-4246-AA73-C343E0FDF1A2}">
+  <dimension ref="A1:M24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="49.33203125" customWidth="1"/>
+    <col min="3" max="3" width="50.88671875" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="3" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" customWidth="1"/>
+    <col min="9" max="9" width="6" customWidth="1"/>
+    <col min="10" max="10" width="13.21875" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>187</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>187</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>187</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>187</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18">
+        <v>184202</v>
+      </c>
+      <c r="D18">
+        <v>198070</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="2">
+        <v>184528</v>
+      </c>
+      <c r="D19" s="2">
+        <v>184538</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>75</v>
+      </c>
+      <c r="G19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H19" t="s">
+        <v>85</v>
+      </c>
+      <c r="I19" t="s">
+        <v>66</v>
+      </c>
+      <c r="J19" t="s">
+        <v>86</v>
+      </c>
+      <c r="K19" t="s">
+        <v>68</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="2">
+        <v>185327</v>
+      </c>
+      <c r="D20" s="2">
+        <v>185350</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>88</v>
+      </c>
+      <c r="G20" t="s">
+        <v>64</v>
+      </c>
+      <c r="H20" t="s">
+        <v>85</v>
+      </c>
+      <c r="I20" t="s">
+        <v>66</v>
+      </c>
+      <c r="J20" t="s">
+        <v>86</v>
+      </c>
+      <c r="K20" t="s">
+        <v>68</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="2">
+        <v>185826</v>
+      </c>
+      <c r="D21" s="2">
+        <v>185936</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>89</v>
+      </c>
+      <c r="G21" t="s">
+        <v>64</v>
+      </c>
+      <c r="H21" t="s">
+        <v>85</v>
+      </c>
+      <c r="I21" t="s">
+        <v>66</v>
+      </c>
+      <c r="J21" t="s">
+        <v>86</v>
+      </c>
+      <c r="K21" t="s">
+        <v>68</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="2">
+        <v>186635</v>
+      </c>
+      <c r="D22" s="2">
+        <v>186916</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>90</v>
+      </c>
+      <c r="G22" t="s">
+        <v>64</v>
+      </c>
+      <c r="H22" t="s">
+        <v>85</v>
+      </c>
+      <c r="I22" t="s">
+        <v>66</v>
+      </c>
+      <c r="J22" t="s">
+        <v>86</v>
+      </c>
+      <c r="K22" t="s">
+        <v>68</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="2">
+        <v>189157</v>
+      </c>
+      <c r="D23" s="2">
+        <v>189426</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>91</v>
+      </c>
+      <c r="G23" t="s">
+        <v>64</v>
+      </c>
+      <c r="H23" t="s">
+        <v>85</v>
+      </c>
+      <c r="I23" t="s">
+        <v>66</v>
+      </c>
+      <c r="J23" t="s">
+        <v>86</v>
+      </c>
+      <c r="K23" t="s">
+        <v>68</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="2">
+        <v>197421</v>
+      </c>
+      <c r="D24" s="2">
+        <v>197520</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>92</v>
+      </c>
+      <c r="G24" t="s">
+        <v>64</v>
+      </c>
+      <c r="H24" t="s">
+        <v>85</v>
+      </c>
+      <c r="I24" t="s">
+        <v>66</v>
+      </c>
+      <c r="J24" t="s">
+        <v>86</v>
+      </c>
+      <c r="K24" t="s">
+        <v>68</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A578C60E-2799-49EC-868F-8AE6684282F0}">
+  <dimension ref="A1:M86"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="51.21875" customWidth="1"/>
+    <col min="12" max="12" width="13.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1">
+        <v>67839</v>
+      </c>
+      <c r="D1">
+        <v>73549</v>
+      </c>
+      <c r="E1">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2">
+        <v>68198</v>
+      </c>
+      <c r="D2">
+        <v>68279</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K2" t="s">
+        <v>68</v>
+      </c>
+      <c r="L2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>70693</v>
+      </c>
+      <c r="D3">
+        <v>70938</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J3" t="s">
+        <v>67</v>
+      </c>
+      <c r="K3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4">
+        <v>71430</v>
+      </c>
+      <c r="D4">
+        <v>71711</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K4" t="s">
+        <v>68</v>
+      </c>
+      <c r="L4" t="s">
+        <v>69</v>
+      </c>
+      <c r="M4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5">
+        <v>72001</v>
+      </c>
+      <c r="D5">
+        <v>72152</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" t="s">
+        <v>66</v>
+      </c>
+      <c r="J5" t="s">
+        <v>67</v>
+      </c>
+      <c r="K5" t="s">
+        <v>68</v>
+      </c>
+      <c r="L5" t="s">
+        <v>69</v>
+      </c>
+      <c r="M5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6">
+        <v>120307</v>
+      </c>
+      <c r="D6">
+        <v>133894</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>120874</v>
+      </c>
+      <c r="D7">
+        <v>120884</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" t="s">
+        <v>76</v>
+      </c>
+      <c r="I7" t="s">
+        <v>66</v>
+      </c>
+      <c r="J7" t="s">
+        <v>77</v>
+      </c>
+      <c r="K7" t="s">
+        <v>68</v>
+      </c>
+      <c r="L7" t="s">
+        <v>78</v>
+      </c>
+      <c r="M7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8">
+        <v>121684</v>
+      </c>
+      <c r="D8">
+        <v>121707</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" t="s">
+        <v>76</v>
+      </c>
+      <c r="I8" t="s">
+        <v>66</v>
+      </c>
+      <c r="J8" t="s">
+        <v>77</v>
+      </c>
+      <c r="K8" t="s">
+        <v>68</v>
+      </c>
+      <c r="L8" t="s">
+        <v>78</v>
+      </c>
+      <c r="M8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9">
+        <v>122181</v>
+      </c>
+      <c r="D9">
+        <v>122291</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" t="s">
+        <v>76</v>
+      </c>
+      <c r="I9" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" t="s">
+        <v>77</v>
+      </c>
+      <c r="K9" t="s">
+        <v>68</v>
+      </c>
+      <c r="L9" t="s">
+        <v>78</v>
+      </c>
+      <c r="M9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10">
+        <v>122976</v>
+      </c>
+      <c r="D10">
+        <v>123257</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H10" t="s">
+        <v>76</v>
+      </c>
+      <c r="I10" t="s">
+        <v>66</v>
+      </c>
+      <c r="J10" t="s">
+        <v>77</v>
+      </c>
+      <c r="K10" t="s">
+        <v>68</v>
+      </c>
+      <c r="L10" t="s">
+        <v>78</v>
+      </c>
+      <c r="M10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>125560</v>
+      </c>
+      <c r="D11">
+        <v>125829</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>82</v>
+      </c>
+      <c r="G11" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" t="s">
+        <v>66</v>
+      </c>
+      <c r="J11" t="s">
+        <v>77</v>
+      </c>
+      <c r="K11" t="s">
+        <v>68</v>
+      </c>
+      <c r="L11" t="s">
+        <v>78</v>
+      </c>
+      <c r="M11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>133482</v>
+      </c>
+      <c r="D12">
+        <v>133581</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" t="s">
+        <v>76</v>
+      </c>
+      <c r="I12" t="s">
+        <v>66</v>
+      </c>
+      <c r="J12" t="s">
+        <v>77</v>
+      </c>
+      <c r="K12" t="s">
+        <v>68</v>
+      </c>
+      <c r="L12" t="s">
+        <v>78</v>
+      </c>
+      <c r="M12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13">
+        <v>184202</v>
+      </c>
+      <c r="D13">
+        <v>198070</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <v>184528</v>
+      </c>
+      <c r="D14">
+        <v>184538</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" t="s">
+        <v>64</v>
+      </c>
+      <c r="H14" t="s">
+        <v>85</v>
+      </c>
+      <c r="I14" t="s">
+        <v>66</v>
+      </c>
+      <c r="J14" t="s">
+        <v>86</v>
+      </c>
+      <c r="K14" t="s">
+        <v>68</v>
+      </c>
+      <c r="L14" t="s">
+        <v>87</v>
+      </c>
+      <c r="M14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15">
+        <v>185327</v>
+      </c>
+      <c r="D15">
+        <v>185350</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" t="s">
+        <v>85</v>
+      </c>
+      <c r="I15" t="s">
+        <v>66</v>
+      </c>
+      <c r="J15" t="s">
+        <v>86</v>
+      </c>
+      <c r="K15" t="s">
+        <v>68</v>
+      </c>
+      <c r="L15" t="s">
+        <v>87</v>
+      </c>
+      <c r="M15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16">
+        <v>185826</v>
+      </c>
+      <c r="D16">
+        <v>185936</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>89</v>
+      </c>
+      <c r="G16" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" t="s">
+        <v>85</v>
+      </c>
+      <c r="I16" t="s">
+        <v>66</v>
+      </c>
+      <c r="J16" t="s">
+        <v>86</v>
+      </c>
+      <c r="K16" t="s">
+        <v>68</v>
+      </c>
+      <c r="L16" t="s">
+        <v>87</v>
+      </c>
+      <c r="M16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17">
+        <v>186635</v>
+      </c>
+      <c r="D17">
+        <v>186916</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>90</v>
+      </c>
+      <c r="G17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H17" t="s">
+        <v>85</v>
+      </c>
+      <c r="I17" t="s">
+        <v>66</v>
+      </c>
+      <c r="J17" t="s">
+        <v>86</v>
+      </c>
+      <c r="K17" t="s">
+        <v>68</v>
+      </c>
+      <c r="L17" t="s">
+        <v>87</v>
+      </c>
+      <c r="M17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18">
+        <v>189157</v>
+      </c>
+      <c r="D18">
+        <v>189426</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" t="s">
+        <v>64</v>
+      </c>
+      <c r="H18" t="s">
+        <v>85</v>
+      </c>
+      <c r="I18" t="s">
+        <v>66</v>
+      </c>
+      <c r="J18" t="s">
+        <v>86</v>
+      </c>
+      <c r="K18" t="s">
+        <v>68</v>
+      </c>
+      <c r="L18" t="s">
+        <v>87</v>
+      </c>
+      <c r="M18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19">
+        <v>197421</v>
+      </c>
+      <c r="D19">
+        <v>197520</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H19" t="s">
+        <v>85</v>
+      </c>
+      <c r="I19" t="s">
+        <v>66</v>
+      </c>
+      <c r="J19" t="s">
+        <v>86</v>
+      </c>
+      <c r="K19" t="s">
+        <v>68</v>
+      </c>
+      <c r="L19" t="s">
+        <v>87</v>
+      </c>
+      <c r="M19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20">
+        <v>240943</v>
+      </c>
+      <c r="D20">
+        <v>247471</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21">
+        <v>241685</v>
+      </c>
+      <c r="D21">
+        <v>241766</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>94</v>
+      </c>
+      <c r="G21" t="s">
+        <v>64</v>
+      </c>
+      <c r="H21" t="s">
+        <v>95</v>
+      </c>
+      <c r="I21" t="s">
+        <v>66</v>
+      </c>
+      <c r="J21" t="s">
+        <v>96</v>
+      </c>
+      <c r="K21" t="s">
+        <v>68</v>
+      </c>
+      <c r="L21" t="s">
+        <v>97</v>
+      </c>
+      <c r="M21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22">
+        <v>245586</v>
+      </c>
+      <c r="D22">
+        <v>245831</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>98</v>
+      </c>
+      <c r="G22" t="s">
+        <v>64</v>
+      </c>
+      <c r="H22" t="s">
+        <v>95</v>
+      </c>
+      <c r="I22" t="s">
+        <v>66</v>
+      </c>
+      <c r="J22" t="s">
+        <v>96</v>
+      </c>
+      <c r="K22" t="s">
+        <v>68</v>
+      </c>
+      <c r="L22" t="s">
+        <v>97</v>
+      </c>
+      <c r="M22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23">
+        <v>246244</v>
+      </c>
+      <c r="D23">
+        <v>246525</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>99</v>
+      </c>
+      <c r="G23" t="s">
+        <v>64</v>
+      </c>
+      <c r="H23" t="s">
+        <v>95</v>
+      </c>
+      <c r="I23" t="s">
+        <v>66</v>
+      </c>
+      <c r="J23" t="s">
+        <v>96</v>
+      </c>
+      <c r="K23" t="s">
+        <v>68</v>
+      </c>
+      <c r="L23" t="s">
+        <v>97</v>
+      </c>
+      <c r="M23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24">
+        <v>246889</v>
+      </c>
+      <c r="D24">
+        <v>247040</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>100</v>
+      </c>
+      <c r="G24" t="s">
+        <v>64</v>
+      </c>
+      <c r="H24" t="s">
+        <v>95</v>
+      </c>
+      <c r="I24" t="s">
+        <v>66</v>
+      </c>
+      <c r="J24" t="s">
+        <v>96</v>
+      </c>
+      <c r="K24" t="s">
+        <v>68</v>
+      </c>
+      <c r="L24" t="s">
+        <v>97</v>
+      </c>
+      <c r="M24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25">
+        <v>259134</v>
+      </c>
+      <c r="D25">
+        <v>266613</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>259343</v>
+      </c>
+      <c r="D26">
+        <v>259353</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>102</v>
+      </c>
+      <c r="G26" t="s">
+        <v>64</v>
+      </c>
+      <c r="H26" t="s">
+        <v>103</v>
+      </c>
+      <c r="I26" t="s">
+        <v>66</v>
+      </c>
+      <c r="J26" t="s">
+        <v>104</v>
+      </c>
+      <c r="K26" t="s">
+        <v>68</v>
+      </c>
+      <c r="L26" t="s">
+        <v>105</v>
+      </c>
+      <c r="M26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27">
+        <v>260474</v>
+      </c>
+      <c r="D27">
+        <v>260584</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>106</v>
+      </c>
+      <c r="G27" t="s">
+        <v>64</v>
+      </c>
+      <c r="H27" t="s">
+        <v>103</v>
+      </c>
+      <c r="I27" t="s">
+        <v>66</v>
+      </c>
+      <c r="J27" t="s">
+        <v>104</v>
+      </c>
+      <c r="K27" t="s">
+        <v>68</v>
+      </c>
+      <c r="L27" t="s">
+        <v>105</v>
+      </c>
+      <c r="M27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28">
+        <v>261101</v>
+      </c>
+      <c r="D28">
+        <v>261382</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
+        <v>107</v>
+      </c>
+      <c r="G28" t="s">
+        <v>64</v>
+      </c>
+      <c r="H28" t="s">
+        <v>103</v>
+      </c>
+      <c r="I28" t="s">
+        <v>66</v>
+      </c>
+      <c r="J28" t="s">
+        <v>104</v>
+      </c>
+      <c r="K28" t="s">
+        <v>68</v>
+      </c>
+      <c r="L28" t="s">
+        <v>105</v>
+      </c>
+      <c r="M28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29">
+        <v>264272</v>
+      </c>
+      <c r="D29">
+        <v>264541</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
+        <v>108</v>
+      </c>
+      <c r="G29" t="s">
+        <v>64</v>
+      </c>
+      <c r="H29" t="s">
+        <v>103</v>
+      </c>
+      <c r="I29" t="s">
+        <v>66</v>
+      </c>
+      <c r="J29" t="s">
+        <v>104</v>
+      </c>
+      <c r="K29" t="s">
+        <v>68</v>
+      </c>
+      <c r="L29" t="s">
+        <v>105</v>
+      </c>
+      <c r="M29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30">
+        <v>265980</v>
+      </c>
+      <c r="D30">
+        <v>266088</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30" t="s">
+        <v>109</v>
+      </c>
+      <c r="G30" t="s">
+        <v>64</v>
+      </c>
+      <c r="H30" t="s">
+        <v>103</v>
+      </c>
+      <c r="I30" t="s">
+        <v>66</v>
+      </c>
+      <c r="J30" t="s">
+        <v>104</v>
+      </c>
+      <c r="K30" t="s">
+        <v>68</v>
+      </c>
+      <c r="L30" t="s">
+        <v>105</v>
+      </c>
+      <c r="M30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31">
+        <v>340828</v>
+      </c>
+      <c r="D31">
+        <v>346703</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32">
+        <v>340908</v>
+      </c>
+      <c r="D32">
+        <v>340989</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>111</v>
+      </c>
+      <c r="G32" t="s">
+        <v>64</v>
+      </c>
+      <c r="H32" t="s">
+        <v>112</v>
+      </c>
+      <c r="I32" t="s">
+        <v>66</v>
+      </c>
+      <c r="J32" t="s">
+        <v>113</v>
+      </c>
+      <c r="K32" t="s">
+        <v>68</v>
+      </c>
+      <c r="L32" t="s">
+        <v>114</v>
+      </c>
+      <c r="M32" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33">
+        <v>344634</v>
+      </c>
+      <c r="D33">
+        <v>344882</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33" t="s">
+        <v>115</v>
+      </c>
+      <c r="G33" t="s">
+        <v>64</v>
+      </c>
+      <c r="H33" t="s">
+        <v>112</v>
+      </c>
+      <c r="I33" t="s">
+        <v>66</v>
+      </c>
+      <c r="J33" t="s">
+        <v>113</v>
+      </c>
+      <c r="K33" t="s">
+        <v>68</v>
+      </c>
+      <c r="L33" t="s">
+        <v>114</v>
+      </c>
+      <c r="M33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34">
+        <v>345266</v>
+      </c>
+      <c r="D34">
+        <v>345547</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>116</v>
+      </c>
+      <c r="G34" t="s">
+        <v>64</v>
+      </c>
+      <c r="H34" t="s">
+        <v>112</v>
+      </c>
+      <c r="I34" t="s">
+        <v>66</v>
+      </c>
+      <c r="J34" t="s">
+        <v>113</v>
+      </c>
+      <c r="K34" t="s">
+        <v>68</v>
+      </c>
+      <c r="L34" t="s">
+        <v>114</v>
+      </c>
+      <c r="M34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35">
+        <v>345715</v>
+      </c>
+      <c r="D35">
+        <v>345866</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35" t="s">
+        <v>117</v>
+      </c>
+      <c r="G35" t="s">
+        <v>64</v>
+      </c>
+      <c r="H35" t="s">
+        <v>112</v>
+      </c>
+      <c r="I35" t="s">
+        <v>66</v>
+      </c>
+      <c r="J35" t="s">
+        <v>113</v>
+      </c>
+      <c r="K35" t="s">
+        <v>68</v>
+      </c>
+      <c r="L35" t="s">
+        <v>114</v>
+      </c>
+      <c r="M35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36">
+        <v>355753</v>
+      </c>
+      <c r="D36">
+        <v>363118</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37">
+        <v>355957</v>
+      </c>
+      <c r="D37">
+        <v>355967</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37" t="s">
+        <v>119</v>
+      </c>
+      <c r="G37" t="s">
+        <v>64</v>
+      </c>
+      <c r="H37" t="s">
+        <v>120</v>
+      </c>
+      <c r="I37" t="s">
+        <v>66</v>
+      </c>
+      <c r="J37" t="s">
+        <v>121</v>
+      </c>
+      <c r="K37" t="s">
+        <v>68</v>
+      </c>
+      <c r="L37" t="s">
+        <v>122</v>
+      </c>
+      <c r="M37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38">
+        <v>356784</v>
+      </c>
+      <c r="D38">
+        <v>356807</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" t="s">
+        <v>123</v>
+      </c>
+      <c r="G38" t="s">
+        <v>64</v>
+      </c>
+      <c r="H38" t="s">
+        <v>120</v>
+      </c>
+      <c r="I38" t="s">
+        <v>66</v>
+      </c>
+      <c r="J38" t="s">
+        <v>121</v>
+      </c>
+      <c r="K38" t="s">
+        <v>68</v>
+      </c>
+      <c r="L38" t="s">
+        <v>122</v>
+      </c>
+      <c r="M38" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39">
+        <v>357277</v>
+      </c>
+      <c r="D39">
+        <v>357387</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39" t="s">
+        <v>124</v>
+      </c>
+      <c r="G39" t="s">
+        <v>64</v>
+      </c>
+      <c r="H39" t="s">
+        <v>120</v>
+      </c>
+      <c r="I39" t="s">
+        <v>66</v>
+      </c>
+      <c r="J39" t="s">
+        <v>121</v>
+      </c>
+      <c r="K39" t="s">
+        <v>68</v>
+      </c>
+      <c r="L39" t="s">
+        <v>122</v>
+      </c>
+      <c r="M39" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40">
+        <v>358355</v>
+      </c>
+      <c r="D40">
+        <v>358636</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40" t="s">
+        <v>125</v>
+      </c>
+      <c r="G40" t="s">
+        <v>64</v>
+      </c>
+      <c r="H40" t="s">
+        <v>120</v>
+      </c>
+      <c r="I40" t="s">
+        <v>66</v>
+      </c>
+      <c r="J40" t="s">
+        <v>121</v>
+      </c>
+      <c r="K40" t="s">
+        <v>68</v>
+      </c>
+      <c r="L40" t="s">
+        <v>122</v>
+      </c>
+      <c r="M40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41">
+        <v>361164</v>
+      </c>
+      <c r="D41">
+        <v>361430</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41" t="s">
+        <v>126</v>
+      </c>
+      <c r="G41" t="s">
+        <v>64</v>
+      </c>
+      <c r="H41" t="s">
+        <v>120</v>
+      </c>
+      <c r="I41" t="s">
+        <v>66</v>
+      </c>
+      <c r="J41" t="s">
+        <v>121</v>
+      </c>
+      <c r="K41" t="s">
+        <v>68</v>
+      </c>
+      <c r="L41" t="s">
+        <v>122</v>
+      </c>
+      <c r="M41" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42">
+        <v>362878</v>
+      </c>
+      <c r="D42">
+        <v>362986</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42" t="s">
+        <v>127</v>
+      </c>
+      <c r="G42" t="s">
+        <v>64</v>
+      </c>
+      <c r="H42" t="s">
+        <v>120</v>
+      </c>
+      <c r="I42" t="s">
+        <v>66</v>
+      </c>
+      <c r="J42" t="s">
+        <v>121</v>
+      </c>
+      <c r="K42" t="s">
+        <v>68</v>
+      </c>
+      <c r="L42" t="s">
+        <v>122</v>
+      </c>
+      <c r="M42" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43">
+        <v>412715</v>
+      </c>
+      <c r="D43">
+        <v>416563</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44">
+        <v>412721</v>
+      </c>
+      <c r="D44">
+        <v>412753</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44" t="s">
+        <v>129</v>
+      </c>
+      <c r="G44" t="s">
+        <v>64</v>
+      </c>
+      <c r="H44" t="s">
+        <v>130</v>
+      </c>
+      <c r="I44" t="s">
+        <v>66</v>
+      </c>
+      <c r="J44" t="s">
+        <v>131</v>
+      </c>
+      <c r="K44" t="s">
+        <v>68</v>
+      </c>
+      <c r="L44" t="s">
+        <v>132</v>
+      </c>
+      <c r="M44" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45">
+        <v>412942</v>
+      </c>
+      <c r="D45">
+        <v>412973</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45" t="s">
+        <v>133</v>
+      </c>
+      <c r="G45" t="s">
+        <v>64</v>
+      </c>
+      <c r="H45" t="s">
+        <v>130</v>
+      </c>
+      <c r="I45" t="s">
+        <v>66</v>
+      </c>
+      <c r="J45" t="s">
+        <v>131</v>
+      </c>
+      <c r="K45" t="s">
+        <v>68</v>
+      </c>
+      <c r="L45" t="s">
+        <v>132</v>
+      </c>
+      <c r="M45" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46">
+        <v>413225</v>
+      </c>
+      <c r="D46">
+        <v>413335</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46" t="s">
+        <v>134</v>
+      </c>
+      <c r="G46" t="s">
+        <v>64</v>
+      </c>
+      <c r="H46" t="s">
+        <v>130</v>
+      </c>
+      <c r="I46" t="s">
+        <v>66</v>
+      </c>
+      <c r="J46" t="s">
+        <v>131</v>
+      </c>
+      <c r="K46" t="s">
+        <v>68</v>
+      </c>
+      <c r="L46" t="s">
+        <v>132</v>
+      </c>
+      <c r="M46" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>60</v>
+      </c>
+      <c r="B47" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47">
+        <v>413822</v>
+      </c>
+      <c r="D47">
+        <v>414103</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47" t="s">
+        <v>135</v>
+      </c>
+      <c r="G47" t="s">
+        <v>64</v>
+      </c>
+      <c r="H47" t="s">
+        <v>130</v>
+      </c>
+      <c r="I47" t="s">
+        <v>66</v>
+      </c>
+      <c r="J47" t="s">
+        <v>131</v>
+      </c>
+      <c r="K47" t="s">
+        <v>68</v>
+      </c>
+      <c r="L47" t="s">
+        <v>132</v>
+      </c>
+      <c r="M47" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>60</v>
+      </c>
+      <c r="B48" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48">
+        <v>414546</v>
+      </c>
+      <c r="D48">
+        <v>414815</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" t="s">
+        <v>136</v>
+      </c>
+      <c r="G48" t="s">
+        <v>64</v>
+      </c>
+      <c r="H48" t="s">
+        <v>130</v>
+      </c>
+      <c r="I48" t="s">
+        <v>66</v>
+      </c>
+      <c r="J48" t="s">
+        <v>131</v>
+      </c>
+      <c r="K48" t="s">
+        <v>68</v>
+      </c>
+      <c r="L48" t="s">
+        <v>132</v>
+      </c>
+      <c r="M48" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>60</v>
+      </c>
+      <c r="B49" t="s">
+        <v>25</v>
+      </c>
+      <c r="C49">
+        <v>416363</v>
+      </c>
+      <c r="D49">
+        <v>416453</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49" t="s">
+        <v>137</v>
+      </c>
+      <c r="G49" t="s">
+        <v>64</v>
+      </c>
+      <c r="H49" t="s">
+        <v>130</v>
+      </c>
+      <c r="I49" t="s">
+        <v>66</v>
+      </c>
+      <c r="J49" t="s">
+        <v>131</v>
+      </c>
+      <c r="K49" t="s">
+        <v>68</v>
+      </c>
+      <c r="L49" t="s">
+        <v>132</v>
+      </c>
+      <c r="M49" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>60</v>
+      </c>
+      <c r="B50" t="s">
+        <v>61</v>
+      </c>
+      <c r="C50">
+        <v>427925</v>
+      </c>
+      <c r="D50">
+        <v>438532</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51" t="s">
+        <v>25</v>
+      </c>
+      <c r="C51">
+        <v>428410</v>
+      </c>
+      <c r="D51">
+        <v>428535</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51" t="s">
+        <v>139</v>
+      </c>
+      <c r="G51" t="s">
+        <v>64</v>
+      </c>
+      <c r="H51" t="s">
+        <v>140</v>
+      </c>
+      <c r="I51" t="s">
+        <v>66</v>
+      </c>
+      <c r="J51" t="s">
+        <v>141</v>
+      </c>
+      <c r="K51" t="s">
+        <v>68</v>
+      </c>
+      <c r="L51" t="s">
+        <v>142</v>
+      </c>
+      <c r="M51" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52" t="s">
+        <v>25</v>
+      </c>
+      <c r="C52">
+        <v>428901</v>
+      </c>
+      <c r="D52">
+        <v>429037</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" t="s">
+        <v>143</v>
+      </c>
+      <c r="G52" t="s">
+        <v>64</v>
+      </c>
+      <c r="H52" t="s">
+        <v>140</v>
+      </c>
+      <c r="I52" t="s">
+        <v>66</v>
+      </c>
+      <c r="J52" t="s">
+        <v>141</v>
+      </c>
+      <c r="K52" t="s">
+        <v>68</v>
+      </c>
+      <c r="L52" t="s">
+        <v>142</v>
+      </c>
+      <c r="M52" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53" t="s">
+        <v>25</v>
+      </c>
+      <c r="C53">
+        <v>429431</v>
+      </c>
+      <c r="D53">
+        <v>429590</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53" t="s">
+        <v>144</v>
+      </c>
+      <c r="G53" t="s">
+        <v>64</v>
+      </c>
+      <c r="H53" t="s">
+        <v>140</v>
+      </c>
+      <c r="I53" t="s">
+        <v>66</v>
+      </c>
+      <c r="J53" t="s">
+        <v>141</v>
+      </c>
+      <c r="K53" t="s">
+        <v>68</v>
+      </c>
+      <c r="L53" t="s">
+        <v>142</v>
+      </c>
+      <c r="M53" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>60</v>
+      </c>
+      <c r="B54" t="s">
+        <v>25</v>
+      </c>
+      <c r="C54">
+        <v>429768</v>
+      </c>
+      <c r="D54">
+        <v>429941</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54" t="s">
+        <v>145</v>
+      </c>
+      <c r="G54" t="s">
+        <v>64</v>
+      </c>
+      <c r="H54" t="s">
+        <v>140</v>
+      </c>
+      <c r="I54" t="s">
+        <v>66</v>
+      </c>
+      <c r="J54" t="s">
+        <v>141</v>
+      </c>
+      <c r="K54" t="s">
+        <v>68</v>
+      </c>
+      <c r="L54" t="s">
+        <v>142</v>
+      </c>
+      <c r="M54" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>60</v>
+      </c>
+      <c r="B55" t="s">
+        <v>25</v>
+      </c>
+      <c r="C55">
+        <v>430119</v>
+      </c>
+      <c r="D55">
+        <v>430307</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55" t="s">
+        <v>146</v>
+      </c>
+      <c r="G55" t="s">
+        <v>64</v>
+      </c>
+      <c r="H55" t="s">
+        <v>140</v>
+      </c>
+      <c r="I55" t="s">
+        <v>66</v>
+      </c>
+      <c r="J55" t="s">
+        <v>141</v>
+      </c>
+      <c r="K55" t="s">
+        <v>68</v>
+      </c>
+      <c r="L55" t="s">
+        <v>142</v>
+      </c>
+      <c r="M55" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>60</v>
+      </c>
+      <c r="B56" t="s">
+        <v>25</v>
+      </c>
+      <c r="C56">
+        <v>431834</v>
+      </c>
+      <c r="D56">
+        <v>431962</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56" t="s">
+        <v>147</v>
+      </c>
+      <c r="G56" t="s">
+        <v>64</v>
+      </c>
+      <c r="H56" t="s">
+        <v>140</v>
+      </c>
+      <c r="I56" t="s">
+        <v>66</v>
+      </c>
+      <c r="J56" t="s">
+        <v>141</v>
+      </c>
+      <c r="K56" t="s">
+        <v>68</v>
+      </c>
+      <c r="L56" t="s">
+        <v>142</v>
+      </c>
+      <c r="M56" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" t="s">
+        <v>25</v>
+      </c>
+      <c r="C57">
+        <v>432128</v>
+      </c>
+      <c r="D57">
+        <v>432325</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57" t="s">
+        <v>148</v>
+      </c>
+      <c r="G57" t="s">
+        <v>64</v>
+      </c>
+      <c r="H57" t="s">
+        <v>140</v>
+      </c>
+      <c r="I57" t="s">
+        <v>66</v>
+      </c>
+      <c r="J57" t="s">
+        <v>141</v>
+      </c>
+      <c r="K57" t="s">
+        <v>68</v>
+      </c>
+      <c r="L57" t="s">
+        <v>142</v>
+      </c>
+      <c r="M57" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" t="s">
+        <v>25</v>
+      </c>
+      <c r="C58">
+        <v>434655</v>
+      </c>
+      <c r="D58">
+        <v>434860</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58" t="s">
+        <v>149</v>
+      </c>
+      <c r="G58" t="s">
+        <v>64</v>
+      </c>
+      <c r="H58" t="s">
+        <v>140</v>
+      </c>
+      <c r="I58" t="s">
+        <v>66</v>
+      </c>
+      <c r="J58" t="s">
+        <v>141</v>
+      </c>
+      <c r="K58" t="s">
+        <v>68</v>
+      </c>
+      <c r="L58" t="s">
+        <v>142</v>
+      </c>
+      <c r="M58" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>60</v>
+      </c>
+      <c r="B59" t="s">
+        <v>25</v>
+      </c>
+      <c r="C59">
+        <v>435144</v>
+      </c>
+      <c r="D59">
+        <v>435274</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59" t="s">
+        <v>150</v>
+      </c>
+      <c r="G59" t="s">
+        <v>64</v>
+      </c>
+      <c r="H59" t="s">
+        <v>140</v>
+      </c>
+      <c r="I59" t="s">
+        <v>66</v>
+      </c>
+      <c r="J59" t="s">
+        <v>141</v>
+      </c>
+      <c r="K59" t="s">
+        <v>68</v>
+      </c>
+      <c r="L59" t="s">
+        <v>142</v>
+      </c>
+      <c r="M59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" t="s">
+        <v>25</v>
+      </c>
+      <c r="C60">
+        <v>437038</v>
+      </c>
+      <c r="D60">
+        <v>437152</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60" t="s">
+        <v>151</v>
+      </c>
+      <c r="G60" t="s">
+        <v>64</v>
+      </c>
+      <c r="H60" t="s">
+        <v>140</v>
+      </c>
+      <c r="I60" t="s">
+        <v>66</v>
+      </c>
+      <c r="J60" t="s">
+        <v>141</v>
+      </c>
+      <c r="K60" t="s">
+        <v>68</v>
+      </c>
+      <c r="L60" t="s">
+        <v>142</v>
+      </c>
+      <c r="M60" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>25</v>
+      </c>
+      <c r="C61">
+        <v>437242</v>
+      </c>
+      <c r="D61">
+        <v>437734</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61" t="s">
+        <v>152</v>
+      </c>
+      <c r="G61" t="s">
+        <v>64</v>
+      </c>
+      <c r="H61" t="s">
+        <v>140</v>
+      </c>
+      <c r="I61" t="s">
+        <v>66</v>
+      </c>
+      <c r="J61" t="s">
+        <v>141</v>
+      </c>
+      <c r="K61" t="s">
+        <v>68</v>
+      </c>
+      <c r="L61" t="s">
+        <v>142</v>
+      </c>
+      <c r="M61" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>61</v>
+      </c>
+      <c r="C62">
+        <v>444461</v>
+      </c>
+      <c r="D62">
+        <v>453730</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>60</v>
+      </c>
+      <c r="B63" t="s">
+        <v>25</v>
+      </c>
+      <c r="C63">
+        <v>445084</v>
+      </c>
+      <c r="D63">
+        <v>445287</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63" t="s">
+        <v>154</v>
+      </c>
+      <c r="G63" t="s">
+        <v>64</v>
+      </c>
+      <c r="H63" t="s">
+        <v>155</v>
+      </c>
+      <c r="I63" t="s">
+        <v>66</v>
+      </c>
+      <c r="J63" t="s">
+        <v>156</v>
+      </c>
+      <c r="K63" t="s">
+        <v>68</v>
+      </c>
+      <c r="L63" t="s">
+        <v>157</v>
+      </c>
+      <c r="M63" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>60</v>
+      </c>
+      <c r="B64" t="s">
+        <v>25</v>
+      </c>
+      <c r="C64">
+        <v>446570</v>
+      </c>
+      <c r="D64">
+        <v>446706</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64" t="s">
+        <v>158</v>
+      </c>
+      <c r="G64" t="s">
+        <v>64</v>
+      </c>
+      <c r="H64" t="s">
+        <v>155</v>
+      </c>
+      <c r="I64" t="s">
+        <v>66</v>
+      </c>
+      <c r="J64" t="s">
+        <v>156</v>
+      </c>
+      <c r="K64" t="s">
+        <v>68</v>
+      </c>
+      <c r="L64" t="s">
+        <v>157</v>
+      </c>
+      <c r="M64" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>60</v>
+      </c>
+      <c r="B65" t="s">
+        <v>25</v>
+      </c>
+      <c r="C65">
+        <v>447015</v>
+      </c>
+      <c r="D65">
+        <v>447177</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65" t="s">
+        <v>159</v>
+      </c>
+      <c r="G65" t="s">
+        <v>64</v>
+      </c>
+      <c r="H65" t="s">
+        <v>155</v>
+      </c>
+      <c r="I65" t="s">
+        <v>66</v>
+      </c>
+      <c r="J65" t="s">
+        <v>156</v>
+      </c>
+      <c r="K65" t="s">
+        <v>68</v>
+      </c>
+      <c r="L65" t="s">
+        <v>157</v>
+      </c>
+      <c r="M65" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>60</v>
+      </c>
+      <c r="B66" t="s">
+        <v>25</v>
+      </c>
+      <c r="C66">
+        <v>447421</v>
+      </c>
+      <c r="D66">
+        <v>447594</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66" t="s">
+        <v>160</v>
+      </c>
+      <c r="G66" t="s">
+        <v>64</v>
+      </c>
+      <c r="H66" t="s">
+        <v>155</v>
+      </c>
+      <c r="I66" t="s">
+        <v>66</v>
+      </c>
+      <c r="J66" t="s">
+        <v>156</v>
+      </c>
+      <c r="K66" t="s">
+        <v>68</v>
+      </c>
+      <c r="L66" t="s">
+        <v>157</v>
+      </c>
+      <c r="M66" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>60</v>
+      </c>
+      <c r="B67" t="s">
+        <v>25</v>
+      </c>
+      <c r="C67">
+        <v>448154</v>
+      </c>
+      <c r="D67">
+        <v>448342</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67" t="s">
+        <v>161</v>
+      </c>
+      <c r="G67" t="s">
+        <v>64</v>
+      </c>
+      <c r="H67" t="s">
+        <v>155</v>
+      </c>
+      <c r="I67" t="s">
+        <v>66</v>
+      </c>
+      <c r="J67" t="s">
+        <v>156</v>
+      </c>
+      <c r="K67" t="s">
+        <v>68</v>
+      </c>
+      <c r="L67" t="s">
+        <v>157</v>
+      </c>
+      <c r="M67" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>60</v>
+      </c>
+      <c r="B68" t="s">
+        <v>25</v>
+      </c>
+      <c r="C68">
+        <v>448492</v>
+      </c>
+      <c r="D68">
+        <v>448620</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68" t="s">
+        <v>162</v>
+      </c>
+      <c r="G68" t="s">
+        <v>64</v>
+      </c>
+      <c r="H68" t="s">
+        <v>155</v>
+      </c>
+      <c r="I68" t="s">
+        <v>66</v>
+      </c>
+      <c r="J68" t="s">
+        <v>156</v>
+      </c>
+      <c r="K68" t="s">
+        <v>68</v>
+      </c>
+      <c r="L68" t="s">
+        <v>157</v>
+      </c>
+      <c r="M68" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>60</v>
+      </c>
+      <c r="B69" t="s">
+        <v>25</v>
+      </c>
+      <c r="C69">
+        <v>449822</v>
+      </c>
+      <c r="D69">
+        <v>450019</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69" t="s">
+        <v>163</v>
+      </c>
+      <c r="G69" t="s">
+        <v>64</v>
+      </c>
+      <c r="H69" t="s">
+        <v>155</v>
+      </c>
+      <c r="I69" t="s">
+        <v>66</v>
+      </c>
+      <c r="J69" t="s">
+        <v>156</v>
+      </c>
+      <c r="K69" t="s">
+        <v>68</v>
+      </c>
+      <c r="L69" t="s">
+        <v>157</v>
+      </c>
+      <c r="M69" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>60</v>
+      </c>
+      <c r="B70" t="s">
+        <v>25</v>
+      </c>
+      <c r="C70">
+        <v>450446</v>
+      </c>
+      <c r="D70">
+        <v>450651</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70" t="s">
+        <v>164</v>
+      </c>
+      <c r="G70" t="s">
+        <v>64</v>
+      </c>
+      <c r="H70" t="s">
+        <v>155</v>
+      </c>
+      <c r="I70" t="s">
+        <v>66</v>
+      </c>
+      <c r="J70" t="s">
+        <v>156</v>
+      </c>
+      <c r="K70" t="s">
+        <v>68</v>
+      </c>
+      <c r="L70" t="s">
+        <v>157</v>
+      </c>
+      <c r="M70" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>60</v>
+      </c>
+      <c r="B71" t="s">
+        <v>25</v>
+      </c>
+      <c r="C71">
+        <v>451611</v>
+      </c>
+      <c r="D71">
+        <v>451741</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71" t="s">
+        <v>165</v>
+      </c>
+      <c r="G71" t="s">
+        <v>64</v>
+      </c>
+      <c r="H71" t="s">
+        <v>155</v>
+      </c>
+      <c r="I71" t="s">
+        <v>66</v>
+      </c>
+      <c r="J71" t="s">
+        <v>156</v>
+      </c>
+      <c r="K71" t="s">
+        <v>68</v>
+      </c>
+      <c r="L71" t="s">
+        <v>157</v>
+      </c>
+      <c r="M71" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>60</v>
+      </c>
+      <c r="B72" t="s">
+        <v>25</v>
+      </c>
+      <c r="C72">
+        <v>451890</v>
+      </c>
+      <c r="D72">
+        <v>452004</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72" t="s">
+        <v>166</v>
+      </c>
+      <c r="G72" t="s">
+        <v>64</v>
+      </c>
+      <c r="H72" t="s">
+        <v>155</v>
+      </c>
+      <c r="I72" t="s">
+        <v>66</v>
+      </c>
+      <c r="J72" t="s">
+        <v>156</v>
+      </c>
+      <c r="K72" t="s">
+        <v>68</v>
+      </c>
+      <c r="L72" t="s">
+        <v>157</v>
+      </c>
+      <c r="M72" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>60</v>
+      </c>
+      <c r="B73" t="s">
+        <v>25</v>
+      </c>
+      <c r="C73">
+        <v>452541</v>
+      </c>
+      <c r="D73">
+        <v>453138</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73" t="s">
+        <v>167</v>
+      </c>
+      <c r="G73" t="s">
+        <v>64</v>
+      </c>
+      <c r="H73" t="s">
+        <v>155</v>
+      </c>
+      <c r="I73" t="s">
+        <v>66</v>
+      </c>
+      <c r="J73" t="s">
+        <v>156</v>
+      </c>
+      <c r="K73" t="s">
+        <v>68</v>
+      </c>
+      <c r="L73" t="s">
+        <v>157</v>
+      </c>
+      <c r="M73" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>60</v>
+      </c>
+      <c r="B74" t="s">
+        <v>61</v>
+      </c>
+      <c r="C74">
+        <v>534450</v>
+      </c>
+      <c r="D74">
+        <v>540342</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>60</v>
+      </c>
+      <c r="B75" t="s">
+        <v>25</v>
+      </c>
+      <c r="C75">
+        <v>534500</v>
+      </c>
+      <c r="D75">
+        <v>534513</v>
+      </c>
+      <c r="E75">
+        <v>1</v>
+      </c>
+      <c r="F75" t="s">
+        <v>169</v>
+      </c>
+      <c r="G75" t="s">
+        <v>64</v>
+      </c>
+      <c r="H75" t="s">
+        <v>170</v>
+      </c>
+      <c r="I75" t="s">
+        <v>66</v>
+      </c>
+      <c r="J75" t="s">
+        <v>171</v>
+      </c>
+      <c r="K75" t="s">
+        <v>68</v>
+      </c>
+      <c r="L75" t="s">
+        <v>172</v>
+      </c>
+      <c r="M75" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>60</v>
+      </c>
+      <c r="B76" t="s">
+        <v>25</v>
+      </c>
+      <c r="C76">
+        <v>534868</v>
+      </c>
+      <c r="D76">
+        <v>534903</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="F76" t="s">
+        <v>173</v>
+      </c>
+      <c r="G76" t="s">
+        <v>64</v>
+      </c>
+      <c r="H76" t="s">
+        <v>170</v>
+      </c>
+      <c r="I76" t="s">
+        <v>66</v>
+      </c>
+      <c r="J76" t="s">
+        <v>171</v>
+      </c>
+      <c r="K76" t="s">
+        <v>68</v>
+      </c>
+      <c r="L76" t="s">
+        <v>172</v>
+      </c>
+      <c r="M76" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>60</v>
+      </c>
+      <c r="B77" t="s">
+        <v>25</v>
+      </c>
+      <c r="C77">
+        <v>535062</v>
+      </c>
+      <c r="D77">
+        <v>535178</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
+      <c r="F77" t="s">
+        <v>174</v>
+      </c>
+      <c r="G77" t="s">
+        <v>64</v>
+      </c>
+      <c r="H77" t="s">
+        <v>170</v>
+      </c>
+      <c r="I77" t="s">
+        <v>66</v>
+      </c>
+      <c r="J77" t="s">
+        <v>171</v>
+      </c>
+      <c r="K77" t="s">
+        <v>68</v>
+      </c>
+      <c r="L77" t="s">
+        <v>172</v>
+      </c>
+      <c r="M77" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>60</v>
+      </c>
+      <c r="B78" t="s">
+        <v>25</v>
+      </c>
+      <c r="C78">
+        <v>536698</v>
+      </c>
+      <c r="D78">
+        <v>536982</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+      <c r="F78" t="s">
+        <v>175</v>
+      </c>
+      <c r="G78" t="s">
+        <v>64</v>
+      </c>
+      <c r="H78" t="s">
+        <v>170</v>
+      </c>
+      <c r="I78" t="s">
+        <v>66</v>
+      </c>
+      <c r="J78" t="s">
+        <v>171</v>
+      </c>
+      <c r="K78" t="s">
+        <v>68</v>
+      </c>
+      <c r="L78" t="s">
+        <v>172</v>
+      </c>
+      <c r="M78" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>60</v>
+      </c>
+      <c r="B79" t="s">
+        <v>25</v>
+      </c>
+      <c r="C79">
+        <v>538210</v>
+      </c>
+      <c r="D79">
+        <v>538491</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+      <c r="F79" t="s">
+        <v>176</v>
+      </c>
+      <c r="G79" t="s">
+        <v>64</v>
+      </c>
+      <c r="H79" t="s">
+        <v>170</v>
+      </c>
+      <c r="I79" t="s">
+        <v>66</v>
+      </c>
+      <c r="J79" t="s">
+        <v>171</v>
+      </c>
+      <c r="K79" t="s">
+        <v>68</v>
+      </c>
+      <c r="L79" t="s">
+        <v>172</v>
+      </c>
+      <c r="M79" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>60</v>
+      </c>
+      <c r="B80" t="s">
+        <v>25</v>
+      </c>
+      <c r="C80">
+        <v>540279</v>
+      </c>
+      <c r="D80">
+        <v>540333</v>
+      </c>
+      <c r="E80">
+        <v>1</v>
+      </c>
+      <c r="F80" t="s">
+        <v>177</v>
+      </c>
+      <c r="G80" t="s">
+        <v>64</v>
+      </c>
+      <c r="H80" t="s">
+        <v>170</v>
+      </c>
+      <c r="I80" t="s">
+        <v>66</v>
+      </c>
+      <c r="J80" t="s">
+        <v>171</v>
+      </c>
+      <c r="K80" t="s">
+        <v>68</v>
+      </c>
+      <c r="L80" t="s">
+        <v>172</v>
+      </c>
+      <c r="M80" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>60</v>
+      </c>
+      <c r="B81" t="s">
+        <v>61</v>
+      </c>
+      <c r="C81">
+        <v>547977</v>
+      </c>
+      <c r="D81">
+        <v>552878</v>
+      </c>
+      <c r="E81">
+        <v>1</v>
+      </c>
+      <c r="F81" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>60</v>
+      </c>
+      <c r="B82" t="s">
+        <v>25</v>
+      </c>
+      <c r="C82">
+        <v>548395</v>
+      </c>
+      <c r="D82">
+        <v>548396</v>
+      </c>
+      <c r="E82">
+        <v>1</v>
+      </c>
+      <c r="F82" t="s">
+        <v>179</v>
+      </c>
+      <c r="G82" t="s">
+        <v>64</v>
+      </c>
+      <c r="H82" t="s">
+        <v>180</v>
+      </c>
+      <c r="I82" t="s">
+        <v>66</v>
+      </c>
+      <c r="J82" t="s">
+        <v>181</v>
+      </c>
+      <c r="K82" t="s">
+        <v>68</v>
+      </c>
+      <c r="L82" t="s">
+        <v>182</v>
+      </c>
+      <c r="M82" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>60</v>
+      </c>
+      <c r="B83" t="s">
+        <v>25</v>
+      </c>
+      <c r="C83">
+        <v>548799</v>
+      </c>
+      <c r="D83">
+        <v>548927</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+      <c r="F83" t="s">
+        <v>183</v>
+      </c>
+      <c r="G83" t="s">
+        <v>64</v>
+      </c>
+      <c r="H83" t="s">
+        <v>180</v>
+      </c>
+      <c r="I83" t="s">
+        <v>66</v>
+      </c>
+      <c r="J83" t="s">
+        <v>181</v>
+      </c>
+      <c r="K83" t="s">
+        <v>68</v>
+      </c>
+      <c r="L83" t="s">
+        <v>182</v>
+      </c>
+      <c r="M83" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>60</v>
+      </c>
+      <c r="B84" t="s">
+        <v>25</v>
+      </c>
+      <c r="C84">
+        <v>549139</v>
+      </c>
+      <c r="D84">
+        <v>549417</v>
+      </c>
+      <c r="E84">
+        <v>1</v>
+      </c>
+      <c r="F84" t="s">
+        <v>184</v>
+      </c>
+      <c r="G84" t="s">
+        <v>64</v>
+      </c>
+      <c r="H84" t="s">
+        <v>180</v>
+      </c>
+      <c r="I84" t="s">
+        <v>66</v>
+      </c>
+      <c r="J84" t="s">
+        <v>181</v>
+      </c>
+      <c r="K84" t="s">
+        <v>68</v>
+      </c>
+      <c r="L84" t="s">
+        <v>182</v>
+      </c>
+      <c r="M84" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>60</v>
+      </c>
+      <c r="B85" t="s">
+        <v>25</v>
+      </c>
+      <c r="C85">
+        <v>550047</v>
+      </c>
+      <c r="D85">
+        <v>550331</v>
+      </c>
+      <c r="E85">
+        <v>1</v>
+      </c>
+      <c r="F85" t="s">
+        <v>185</v>
+      </c>
+      <c r="G85" t="s">
+        <v>64</v>
+      </c>
+      <c r="H85" t="s">
+        <v>180</v>
+      </c>
+      <c r="I85" t="s">
+        <v>66</v>
+      </c>
+      <c r="J85" t="s">
+        <v>181</v>
+      </c>
+      <c r="K85" t="s">
+        <v>68</v>
+      </c>
+      <c r="L85" t="s">
+        <v>182</v>
+      </c>
+      <c r="M85" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>60</v>
+      </c>
+      <c r="B86" t="s">
+        <v>25</v>
+      </c>
+      <c r="C86">
+        <v>552477</v>
+      </c>
+      <c r="D86">
+        <v>552564</v>
+      </c>
+      <c r="E86">
+        <v>1</v>
+      </c>
+      <c r="F86" t="s">
+        <v>186</v>
+      </c>
+      <c r="G86" t="s">
+        <v>64</v>
+      </c>
+      <c r="H86" t="s">
+        <v>180</v>
+      </c>
+      <c r="I86" t="s">
+        <v>66</v>
+      </c>
+      <c r="J86" t="s">
+        <v>181</v>
+      </c>
+      <c r="K86" t="s">
+        <v>68</v>
+      </c>
+      <c r="L86" t="s">
+        <v>182</v>
+      </c>
+      <c r="M86" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>